<commit_message>
update aesthetics of figures
</commit_message>
<xml_diff>
--- a/figure_table/toyexample_TEMPTED.xlsx
+++ b/figure_table/toyexample_TEMPTED.xlsx
@@ -392,10 +392,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.07880033100398944</v>
+        <v>-0.07880033100398944</v>
       </c>
       <c r="C2">
-        <v>-0.1214369994391653</v>
+        <v>0.1214369994391653</v>
       </c>
       <c r="D2">
         <v>0.08286637801416286</v>
@@ -408,10 +408,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.1597047368379094</v>
+        <v>-0.1597047368379094</v>
       </c>
       <c r="C3">
-        <v>-0.08924064136581804</v>
+        <v>0.08924064136581804</v>
       </c>
       <c r="D3">
         <v>0.02194583339231184</v>
@@ -424,10 +424,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.09182320861932254</v>
+        <v>-0.09182320861932254</v>
       </c>
       <c r="C4">
-        <v>-0.1399065702590379</v>
+        <v>0.1399065702590379</v>
       </c>
       <c r="D4">
         <v>0.08142219514737449</v>
@@ -440,10 +440,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.06885075539748635</v>
+        <v>-0.06885075539748635</v>
       </c>
       <c r="C5">
-        <v>-0.1507682320556845</v>
+        <v>0.1507682320556845</v>
       </c>
       <c r="D5">
         <v>0.1828830105495226</v>
@@ -456,10 +456,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.1064637437162154</v>
+        <v>-0.1064637437162154</v>
       </c>
       <c r="C6">
-        <v>-0.2004787865145692</v>
+        <v>0.2004787865145692</v>
       </c>
       <c r="D6">
         <v>0.1593372006206886</v>
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.08468212103776607</v>
+        <v>-0.08468212103776607</v>
       </c>
       <c r="C7">
-        <v>-0.231414938101536</v>
+        <v>0.231414938101536</v>
       </c>
       <c r="D7">
         <v>0.1374942494335623</v>
@@ -488,10 +488,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.006942093937174086</v>
+        <v>-0.006942093937174086</v>
       </c>
       <c r="C8">
-        <v>-0.1569134902252004</v>
+        <v>0.1569134902252004</v>
       </c>
       <c r="D8">
         <v>0.1709881830670296</v>
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.1181267850122958</v>
+        <v>-0.1181267850122958</v>
       </c>
       <c r="C9">
-        <v>-0.1579221650765876</v>
+        <v>0.1579221650765876</v>
       </c>
       <c r="D9">
         <v>0.08154890345050997</v>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.03989675258009495</v>
+        <v>-0.03989675258009495</v>
       </c>
       <c r="C10">
-        <v>-0.149923486753858</v>
+        <v>0.149923486753858</v>
       </c>
       <c r="D10">
         <v>0.181058889512264</v>
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.03398321206824673</v>
+        <v>-0.03398321206824673</v>
       </c>
       <c r="C11">
-        <v>-0.1325572000438724</v>
+        <v>0.1325572000438724</v>
       </c>
       <c r="D11">
         <v>0.09324971122061536</v>
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.0393834362513036</v>
+        <v>-0.0393834362513036</v>
       </c>
       <c r="C12">
-        <v>-0.1069070723376464</v>
+        <v>0.1069070723376464</v>
       </c>
       <c r="D12">
         <v>0.06029063684868469</v>
@@ -568,10 +568,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.06418415895501667</v>
+        <v>-0.06418415895501667</v>
       </c>
       <c r="C13">
-        <v>-0.1279859881148709</v>
+        <v>0.1279859881148709</v>
       </c>
       <c r="D13">
         <v>0.1195667273895422</v>
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.07242971303684753</v>
+        <v>-0.07242971303684753</v>
       </c>
       <c r="C14">
-        <v>-0.1494128835333963</v>
+        <v>0.1494128835333963</v>
       </c>
       <c r="D14">
         <v>0.04266706133200412</v>
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.09029877826118225</v>
+        <v>-0.09029877826118225</v>
       </c>
       <c r="C15">
-        <v>-0.1625674025572098</v>
+        <v>0.1625674025572098</v>
       </c>
       <c r="D15">
         <v>0.05610808754397775</v>
@@ -616,10 +616,10 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.0326595669318467</v>
+        <v>-0.0326595669318467</v>
       </c>
       <c r="C16">
-        <v>-0.1491304409524304</v>
+        <v>0.1491304409524304</v>
       </c>
       <c r="D16">
         <v>0.08068434163336682</v>
@@ -632,10 +632,10 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.05572218326875031</v>
+        <v>-0.05572218326875031</v>
       </c>
       <c r="C17">
-        <v>-0.1282802804216011</v>
+        <v>0.1282802804216011</v>
       </c>
       <c r="D17">
         <v>0.06982946815661424</v>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.1188887401453342</v>
+        <v>-0.1188887401453342</v>
       </c>
       <c r="C18">
-        <v>-0.196080812070059</v>
+        <v>0.196080812070059</v>
       </c>
       <c r="D18">
         <v>0.08348757761444664</v>
@@ -664,10 +664,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.09593907800657581</v>
+        <v>-0.09593907800657581</v>
       </c>
       <c r="C19">
-        <v>-0.1112069989509569</v>
+        <v>0.1112069989509569</v>
       </c>
       <c r="D19">
         <v>0.2161882178419718</v>
@@ -680,10 +680,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.059080270576451</v>
+        <v>-0.059080270576451</v>
       </c>
       <c r="C20">
-        <v>-0.1287622198577844</v>
+        <v>0.1287622198577844</v>
       </c>
       <c r="D20">
         <v>0.06929104037800883</v>
@@ -696,10 +696,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.1086246116494793</v>
+        <v>-0.1086246116494793</v>
       </c>
       <c r="C21">
-        <v>-0.2478063645090004</v>
+        <v>0.2478063645090004</v>
       </c>
       <c r="D21">
         <v>0.1040687696044373</v>
@@ -712,10 +712,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.1207840450460627</v>
+        <v>-0.1207840450460627</v>
       </c>
       <c r="C22">
-        <v>-0.0400602660338118</v>
+        <v>0.0400602660338118</v>
       </c>
       <c r="D22">
         <v>0.1523271192084657</v>
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.1424967482471836</v>
+        <v>-0.1424967482471836</v>
       </c>
       <c r="C23">
-        <v>0.04804290026338388</v>
+        <v>-0.04804290026338388</v>
       </c>
       <c r="D23">
         <v>0.1215239350647906</v>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.1841318024115703</v>
+        <v>-0.1841318024115703</v>
       </c>
       <c r="C24">
-        <v>-0.05304303404014515</v>
+        <v>0.05304303404014515</v>
       </c>
       <c r="D24">
         <v>0.1052458977956333</v>
@@ -760,10 +760,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.1880883407097291</v>
+        <v>-0.1880883407097291</v>
       </c>
       <c r="C25">
-        <v>-0.04652472903038417</v>
+        <v>0.04652472903038417</v>
       </c>
       <c r="D25">
         <v>0.07786685759590449</v>
@@ -776,10 +776,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.1166535035664137</v>
+        <v>-0.1166535035664137</v>
       </c>
       <c r="C26">
-        <v>-0.05331014115494709</v>
+        <v>0.05331014115494709</v>
       </c>
       <c r="D26">
         <v>0.1084221622006323</v>
@@ -792,10 +792,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.1489222249139132</v>
+        <v>-0.1489222249139132</v>
       </c>
       <c r="C27">
-        <v>-0.01787104103422705</v>
+        <v>0.01787104103422705</v>
       </c>
       <c r="D27">
         <v>0.1304433213087429</v>
@@ -808,10 +808,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.1361027041258603</v>
+        <v>-0.1361027041258603</v>
       </c>
       <c r="C28">
-        <v>0.04405263595672025</v>
+        <v>-0.04405263595672025</v>
       </c>
       <c r="D28">
         <v>0.1052854343647315</v>
@@ -824,10 +824,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.1246603111788643</v>
+        <v>-0.1246603111788643</v>
       </c>
       <c r="C29">
-        <v>0.004160658796581899</v>
+        <v>-0.004160658796581899</v>
       </c>
       <c r="D29">
         <v>0.09807544077649784</v>
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.1574420473153161</v>
+        <v>-0.1574420473153161</v>
       </c>
       <c r="C30">
-        <v>-0.06313717410600292</v>
+        <v>0.06313717410600292</v>
       </c>
       <c r="D30">
         <v>0.1041393907348075</v>
@@ -856,10 +856,10 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.1060189038618903</v>
+        <v>-0.1060189038618903</v>
       </c>
       <c r="C31">
-        <v>-0.08657780365855253</v>
+        <v>0.08657780365855253</v>
       </c>
       <c r="D31">
         <v>0.04694756544500957</v>
@@ -872,10 +872,10 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.1568412589673558</v>
+        <v>-0.1568412589673558</v>
       </c>
       <c r="C32">
-        <v>0.0087038431122955</v>
+        <v>-0.0087038431122955</v>
       </c>
       <c r="D32">
         <v>0.09739018354220523</v>
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.1518207445508232</v>
+        <v>-0.1518207445508232</v>
       </c>
       <c r="C33">
-        <v>-0.01938041579834017</v>
+        <v>0.01938041579834017</v>
       </c>
       <c r="D33">
         <v>0.1035820134209568</v>
@@ -904,10 +904,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.08476183168910413</v>
+        <v>-0.08476183168910413</v>
       </c>
       <c r="C34">
-        <v>0.0488533308951106</v>
+        <v>-0.0488533308951106</v>
       </c>
       <c r="D34">
         <v>0.09051974234979543</v>
@@ -920,10 +920,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.1904791751848131</v>
+        <v>-0.1904791751848131</v>
       </c>
       <c r="C35">
-        <v>0.006666381894677296</v>
+        <v>-0.006666381894677296</v>
       </c>
       <c r="D35">
         <v>0.1115794817294884</v>
@@ -936,10 +936,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.1197296066625953</v>
+        <v>-0.1197296066625953</v>
       </c>
       <c r="C36">
-        <v>0.04137040799836017</v>
+        <v>-0.04137040799836017</v>
       </c>
       <c r="D36">
         <v>0.191588624992434</v>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.09845232729245383</v>
+        <v>-0.09845232729245383</v>
       </c>
       <c r="C37">
-        <v>-0.02353201588609518</v>
+        <v>0.02353201588609518</v>
       </c>
       <c r="D37">
         <v>0.2011007193876927</v>
@@ -968,10 +968,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.1504012091219676</v>
+        <v>-0.1504012091219676</v>
       </c>
       <c r="C38">
-        <v>0.02765697563870612</v>
+        <v>-0.02765697563870612</v>
       </c>
       <c r="D38">
         <v>0.100213658553973</v>
@@ -984,10 +984,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.07122830914109726</v>
+        <v>-0.07122830914109726</v>
       </c>
       <c r="C39">
-        <v>-0.07506640441448975</v>
+        <v>0.07506640441448975</v>
       </c>
       <c r="D39">
         <v>0.2206316210571686</v>
@@ -1000,10 +1000,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.2265197967315946</v>
+        <v>-0.2265197967315946</v>
       </c>
       <c r="C40">
-        <v>0.04740057954479043</v>
+        <v>-0.04740057954479043</v>
       </c>
       <c r="D40">
         <v>0.01361621534738438</v>
@@ -1016,10 +1016,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.1613174140009147</v>
+        <v>-0.1613174140009147</v>
       </c>
       <c r="C41">
-        <v>0.009525502976460364</v>
+        <v>-0.009525502976460364</v>
       </c>
       <c r="D41">
         <v>0.1016482954363994</v>
@@ -1032,10 +1032,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>-0.1524815940947832</v>
+        <v>0.1524815940947832</v>
       </c>
       <c r="C42">
-        <v>-0.09539351800340515</v>
+        <v>0.09539351800340515</v>
       </c>
       <c r="D42">
         <v>0.07907566791150117</v>
@@ -1048,10 +1048,10 @@
         </is>
       </c>
       <c r="B43">
-        <v>-0.1006952260212896</v>
+        <v>0.1006952260212896</v>
       </c>
       <c r="C43">
-        <v>-0.1754087969904064</v>
+        <v>0.1754087969904064</v>
       </c>
       <c r="D43">
         <v>0.1010814514830914</v>
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="B44">
-        <v>-0.1297706116613269</v>
+        <v>0.1297706116613269</v>
       </c>
       <c r="C44">
-        <v>-0.16258805335235</v>
+        <v>0.16258805335235</v>
       </c>
       <c r="D44">
         <v>0.1126153295510959</v>
@@ -1080,10 +1080,10 @@
         </is>
       </c>
       <c r="B45">
-        <v>-0.06887893405855348</v>
+        <v>0.06887893405855348</v>
       </c>
       <c r="C45">
-        <v>-0.2011623620254935</v>
+        <v>0.2011623620254935</v>
       </c>
       <c r="D45">
         <v>0.1052471457489279</v>
@@ -1096,10 +1096,10 @@
         </is>
       </c>
       <c r="B46">
-        <v>-0.1286975011557017</v>
+        <v>0.1286975011557017</v>
       </c>
       <c r="C46">
-        <v>-0.1366386636569925</v>
+        <v>0.1366386636569925</v>
       </c>
       <c r="D46">
         <v>0.1089611643971406</v>
@@ -1112,10 +1112,10 @@
         </is>
       </c>
       <c r="B47">
-        <v>-0.1391387690211929</v>
+        <v>0.1391387690211929</v>
       </c>
       <c r="C47">
-        <v>-0.1430096268577066</v>
+        <v>0.1430096268577066</v>
       </c>
       <c r="D47">
         <v>0.1007542559006574</v>
@@ -1128,10 +1128,10 @@
         </is>
       </c>
       <c r="B48">
-        <v>-0.08871823613264167</v>
+        <v>0.08871823613264167</v>
       </c>
       <c r="C48">
-        <v>-0.2535098651157587</v>
+        <v>0.2535098651157587</v>
       </c>
       <c r="D48">
         <v>0.1150785997162549</v>
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="B49">
-        <v>-0.1877606920033705</v>
+        <v>0.1877606920033705</v>
       </c>
       <c r="C49">
-        <v>-0.1148520871673355</v>
+        <v>0.1148520871673355</v>
       </c>
       <c r="D49">
         <v>0.201843583806864</v>
@@ -1160,10 +1160,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>-0.1569417085128846</v>
+        <v>0.1569417085128846</v>
       </c>
       <c r="C50">
-        <v>-0.1367260694464659</v>
+        <v>0.1367260694464659</v>
       </c>
       <c r="D50">
         <v>0.2812543447786442</v>
@@ -1176,10 +1176,10 @@
         </is>
       </c>
       <c r="B51">
-        <v>-0.1594157473842039</v>
+        <v>0.1594157473842039</v>
       </c>
       <c r="C51">
-        <v>-0.126431634358593</v>
+        <v>0.126431634358593</v>
       </c>
       <c r="D51">
         <v>0.222429672884922</v>
@@ -1192,10 +1192,10 @@
         </is>
       </c>
       <c r="B52">
-        <v>-0.166420343368233</v>
+        <v>0.166420343368233</v>
       </c>
       <c r="C52">
-        <v>-0.1029979520168319</v>
+        <v>0.1029979520168319</v>
       </c>
       <c r="D52">
         <v>0.1730408711989471</v>
@@ -1208,10 +1208,10 @@
         </is>
       </c>
       <c r="B53">
-        <v>-0.1389604624739776</v>
+        <v>0.1389604624739776</v>
       </c>
       <c r="C53">
-        <v>-0.07987778110635416</v>
+        <v>0.07987778110635416</v>
       </c>
       <c r="D53">
         <v>0.07531211867155593</v>
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B54">
-        <v>-0.09480884968176284</v>
+        <v>0.09480884968176284</v>
       </c>
       <c r="C54">
-        <v>-0.136970448380681</v>
+        <v>0.136970448380681</v>
       </c>
       <c r="D54">
         <v>0.1058745716315293</v>
@@ -1240,10 +1240,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>-0.171837564703721</v>
+        <v>0.171837564703721</v>
       </c>
       <c r="C55">
-        <v>-0.1385598712777725</v>
+        <v>0.1385598712777725</v>
       </c>
       <c r="D55">
         <v>0.1060105896373873</v>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>-0.192171193283747</v>
+        <v>0.192171193283747</v>
       </c>
       <c r="C56">
-        <v>-0.1387569041945457</v>
+        <v>0.1387569041945457</v>
       </c>
       <c r="D56">
         <v>0.1729712366942464</v>
@@ -1272,10 +1272,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>-0.2048876041419146</v>
+        <v>0.2048876041419146</v>
       </c>
       <c r="C57">
-        <v>-0.08165555404799489</v>
+        <v>0.08165555404799489</v>
       </c>
       <c r="D57">
         <v>0.1692860454501073</v>
@@ -1288,10 +1288,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>-0.1636535110991047</v>
+        <v>0.1636535110991047</v>
       </c>
       <c r="C58">
-        <v>-0.1410792001829381</v>
+        <v>0.1410792001829381</v>
       </c>
       <c r="D58">
         <v>0.1310094319869677</v>
@@ -1304,10 +1304,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>-0.09529976887725825</v>
+        <v>0.09529976887725825</v>
       </c>
       <c r="C59">
-        <v>-0.1489229712502358</v>
+        <v>0.1489229712502358</v>
       </c>
       <c r="D59">
         <v>0.08593932294132844</v>
@@ -1320,10 +1320,10 @@
         </is>
       </c>
       <c r="B60">
-        <v>-0.1704178216584816</v>
+        <v>0.1704178216584816</v>
       </c>
       <c r="C60">
-        <v>-0.1004813114613144</v>
+        <v>0.1004813114613144</v>
       </c>
       <c r="D60">
         <v>0.09599681296790769</v>
@@ -1336,10 +1336,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>-0.1198211957719144</v>
+        <v>0.1198211957719144</v>
       </c>
       <c r="C61">
-        <v>-0.277698010227947</v>
+        <v>0.277698010227947</v>
       </c>
       <c r="D61">
         <v>0.1649019368160083</v>
@@ -3012,10 +3012,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-0.03584611425551176</v>
+        <v>0.03584611425551176</v>
       </c>
       <c r="B2">
-        <v>0.1261660229675725</v>
+        <v>-0.1261660229675725</v>
       </c>
       <c r="C2">
         <v>-0.2114090648450627</v>
@@ -3023,10 +3023,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>-0.03888348454188601</v>
+        <v>0.03888348454188601</v>
       </c>
       <c r="B3">
-        <v>0.1280966100874439</v>
+        <v>-0.1280966100874439</v>
       </c>
       <c r="C3">
         <v>-0.1908208461452241</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>-0.04190078771077085</v>
+        <v>0.04190078771077085</v>
       </c>
       <c r="B4">
-        <v>0.1300479773889831</v>
+        <v>-0.1300479773889831</v>
       </c>
       <c r="C4">
         <v>-0.1702523380531559</v>
@@ -3045,10 +3045,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>-0.04485766930607214</v>
+        <v>0.04485766930607214</v>
       </c>
       <c r="B5">
-        <v>0.1320303666728868</v>
+        <v>-0.1320303666728868</v>
       </c>
       <c r="C5">
         <v>-0.1497399351875364</v>
@@ -3056,10 +3056,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>-0.04771968755473609</v>
+        <v>0.04771968755473609</v>
       </c>
       <c r="B6">
-        <v>0.1340030946923663</v>
+        <v>-0.1340030946923663</v>
       </c>
       <c r="C6">
         <v>-0.1293541106290052</v>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>-0.05049449189690745</v>
+        <v>0.05049449189690745</v>
       </c>
       <c r="B7">
-        <v>0.1358767400937768</v>
+        <v>-0.1358767400937768</v>
       </c>
       <c r="C7">
         <v>-0.1091667532894945</v>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>-0.05323720007498162</v>
+        <v>0.05323720007498162</v>
       </c>
       <c r="B8">
-        <v>0.1375873429855182</v>
+        <v>-0.1375873429855182</v>
       </c>
       <c r="C8">
         <v>-0.08923731780255828</v>
@@ -3089,10 +3089,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>-0.05602764123582211</v>
+        <v>0.05602764123582211</v>
       </c>
       <c r="B9">
-        <v>0.139112344381051</v>
+        <v>-0.139112344381051</v>
       </c>
       <c r="C9">
         <v>-0.06960621210965814</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>-0.05891856211600118</v>
+        <v>0.05891856211600118</v>
       </c>
       <c r="B10">
-        <v>0.1403709563575088</v>
+        <v>-0.1403709563575088</v>
       </c>
       <c r="C10">
         <v>-0.05037354421408783</v>
@@ -3111,10 +3111,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>-0.06192080305161932</v>
+        <v>0.06192080305161932</v>
       </c>
       <c r="B11">
-        <v>0.1412620094606763</v>
+        <v>-0.1412620094606763</v>
       </c>
       <c r="C11">
         <v>-0.03166623998205532</v>
@@ -3122,10 +3122,10 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>-0.06502997221068191</v>
+        <v>0.06502997221068191</v>
       </c>
       <c r="B12">
-        <v>0.1417049914353085</v>
+        <v>-0.1417049914353085</v>
       </c>
       <c r="C12">
         <v>-0.0136124037126967</v>
@@ -3133,10 +3133,10 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>-0.0682217927374613</v>
+        <v>0.0682217927374613</v>
       </c>
       <c r="B13">
-        <v>0.1417017789286655</v>
+        <v>-0.1417017789286655</v>
       </c>
       <c r="C13">
         <v>0.003655262130591408</v>
@@ -3144,10 +3144,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>-0.07147981864187419</v>
+        <v>0.07147981864187419</v>
       </c>
       <c r="B14">
-        <v>0.1412829067322424</v>
+        <v>-0.1412829067322424</v>
       </c>
       <c r="C14">
         <v>0.02002067260579577</v>
@@ -3155,10 +3155,10 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>-0.07479378898660065</v>
+        <v>0.07479378898660065</v>
       </c>
       <c r="B15">
-        <v>0.1404766937034764</v>
+        <v>-0.1404766937034764</v>
       </c>
       <c r="C15">
         <v>0.03541008150476255</v>
@@ -3166,10 +3166,10 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>-0.07813776785780477</v>
+        <v>0.07813776785780477</v>
       </c>
       <c r="B16">
-        <v>0.1393327134303599</v>
+        <v>-0.1393327134303599</v>
       </c>
       <c r="C16">
         <v>0.04973524646842393</v>
@@ -3177,10 +3177,10 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>-0.0814609933235251</v>
+        <v>0.0814609933235251</v>
       </c>
       <c r="B17">
-        <v>0.1379115473026885</v>
+        <v>-0.1379115473026885</v>
       </c>
       <c r="C17">
         <v>0.06291090653511749</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>-0.0847460889320646</v>
+        <v>0.0847460889320646</v>
       </c>
       <c r="B18">
-        <v>0.1362359448069206</v>
+        <v>-0.1362359448069206</v>
       </c>
       <c r="C18">
         <v>0.07489361441684624</v>
@@ -3199,10 +3199,10 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>-0.08798957340369122</v>
+        <v>0.08798957340369122</v>
       </c>
       <c r="B19">
-        <v>0.13431261277634</v>
+        <v>-0.13431261277634</v>
       </c>
       <c r="C19">
         <v>0.08567338841457367</v>
@@ -3210,10 +3210,10 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>-0.09116892161060079</v>
+        <v>0.09116892161060079</v>
       </c>
       <c r="B20">
-        <v>0.1321639880710429</v>
+        <v>-0.1321639880710429</v>
       </c>
       <c r="C20">
         <v>0.0952191600999244</v>
@@ -3221,10 +3221,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>-0.09425152007691803</v>
+        <v>0.09425152007691803</v>
       </c>
       <c r="B21">
-        <v>0.129792202374663</v>
+        <v>-0.129792202374663</v>
       </c>
       <c r="C21">
         <v>0.1034293501194486</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>-0.09718356612790389</v>
+        <v>0.09718356612790389</v>
       </c>
       <c r="B22">
-        <v>0.1271917421652431</v>
+        <v>-0.1271917421652431</v>
       </c>
       <c r="C22">
         <v>0.1101934723703826</v>
@@ -3243,10 +3243,10 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>-0.0999147371795141</v>
+        <v>0.0999147371795141</v>
       </c>
       <c r="B23">
-        <v>0.1243474336847771</v>
+        <v>-0.1243474336847771</v>
       </c>
       <c r="C23">
         <v>0.1154325310850253</v>
@@ -3254,10 +3254,10 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>-0.1024411458943892</v>
+        <v>0.1024411458943892</v>
       </c>
       <c r="B24">
-        <v>0.1212491236992373</v>
+        <v>-0.1212491236992373</v>
       </c>
       <c r="C24">
         <v>0.1191109387747327</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>-0.104758855565474</v>
+        <v>0.104758855565474</v>
       </c>
       <c r="B25">
-        <v>0.1178570458575076</v>
+        <v>-0.1178570458575076</v>
       </c>
       <c r="C25">
         <v>0.121241093243928</v>
@@ -3276,10 +3276,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>-0.1068821113627917</v>
+        <v>0.1068821113627917</v>
       </c>
       <c r="B26">
-        <v>0.1141234166013049</v>
+        <v>-0.1141234166013049</v>
       </c>
       <c r="C26">
         <v>0.1218533141761865</v>
@@ -3287,10 +3287,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>-0.1088122123022573</v>
+        <v>0.1088122123022573</v>
       </c>
       <c r="B27">
-        <v>0.1100091261522422</v>
+        <v>-0.1100091261522422</v>
       </c>
       <c r="C27">
         <v>0.1210042011080165</v>
@@ -3298,10 +3298,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>-0.1104941612425646</v>
+        <v>0.1104941612425646</v>
       </c>
       <c r="B28">
-        <v>0.1054996126930566</v>
+        <v>-0.1054996126930566</v>
       </c>
       <c r="C28">
         <v>0.1187307541634631</v>
@@ -3309,10 +3309,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>-0.1118783610632255</v>
+        <v>0.1118783610632255</v>
       </c>
       <c r="B29">
-        <v>0.1006290414523116</v>
+        <v>-0.1006290414523116</v>
       </c>
       <c r="C29">
         <v>0.1150658859673596</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>-0.1129648114253242</v>
+        <v>0.1129648114253242</v>
       </c>
       <c r="B30">
-        <v>0.09542311040749513</v>
+        <v>-0.09542311040749513</v>
       </c>
       <c r="C30">
         <v>0.1100693033274244</v>
@@ -3331,10 +3331,10 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>-0.1137631319739484</v>
+        <v>0.1137631319739484</v>
       </c>
       <c r="B31">
-        <v>0.0898902283505609</v>
+        <v>-0.0898902283505609</v>
       </c>
       <c r="C31">
         <v>0.1038190413265975</v>
@@ -3342,10 +3342,10 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>-0.1142600113166586</v>
+        <v>0.1142600113166586</v>
       </c>
       <c r="B32">
-        <v>0.08402796676416481</v>
+        <v>-0.08402796676416481</v>
       </c>
       <c r="C32">
         <v>0.09636623408259679</v>
@@ -3353,10 +3353,10 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>-0.1144563690838302</v>
+        <v>0.1144563690838302</v>
       </c>
       <c r="B33">
-        <v>0.07785485117788461</v>
+        <v>-0.07785485117788461</v>
       </c>
       <c r="C33">
         <v>0.08777310153522087</v>
@@ -3364,10 +3364,10 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>-0.1144043171831065</v>
+        <v>0.1144043171831065</v>
       </c>
       <c r="B34">
-        <v>0.07138520866556547</v>
+        <v>-0.07138520866556547</v>
       </c>
       <c r="C34">
         <v>0.07810488671683126</v>
@@ -3375,10 +3375,10 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>-0.1142021332788516</v>
+        <v>0.1142021332788516</v>
       </c>
       <c r="B35">
-        <v>0.06460178118966367</v>
+        <v>-0.06460178118966367</v>
       </c>
       <c r="C35">
         <v>0.067394993701182</v>
@@ -3386,10 +3386,10 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>-0.1139490195579526</v>
+        <v>0.1139490195579526</v>
       </c>
       <c r="B36">
-        <v>0.05753619880781555</v>
+        <v>-0.05753619880781555</v>
       </c>
       <c r="C36">
         <v>0.05569652325763148</v>
@@ -3397,10 +3397,10 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>-0.1137118752692501</v>
+        <v>0.1137118752692501</v>
       </c>
       <c r="B37">
-        <v>0.05024153762267213</v>
+        <v>-0.05024153762267213</v>
       </c>
       <c r="C37">
         <v>0.04310554140968866</v>
@@ -3408,10 +3408,10 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>-0.1135261950400183</v>
+        <v>0.1135261950400183</v>
       </c>
       <c r="B38">
-        <v>0.0427547203437779</v>
+        <v>-0.0427547203437779</v>
       </c>
       <c r="C38">
         <v>0.02972379916907733</v>
@@ -3419,10 +3419,10 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>-0.1133952595789638</v>
+        <v>0.1133952595789638</v>
       </c>
       <c r="B39">
-        <v>0.03510418176991831</v>
+        <v>-0.03510418176991831</v>
       </c>
       <c r="C39">
         <v>0.01564281432055305</v>
@@ -3430,10 +3430,10 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>-0.1133439230422368</v>
+        <v>0.1133439230422368</v>
       </c>
       <c r="B40">
-        <v>0.02734071614690875</v>
+        <v>-0.02734071614690875</v>
       </c>
       <c r="C40">
         <v>0.0009725763272283479</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>-0.1134246352605632</v>
+        <v>0.1134246352605632</v>
       </c>
       <c r="B41">
-        <v>0.01951218510840367</v>
+        <v>-0.01951218510840367</v>
       </c>
       <c r="C41">
         <v>-0.01414504278215793</v>
@@ -3452,10 +3452,10 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>-0.1136633701498238</v>
+        <v>0.1136633701498238</v>
       </c>
       <c r="B42">
-        <v>0.01164778875484332</v>
+        <v>-0.01164778875484332</v>
       </c>
       <c r="C42">
         <v>-0.02952782495901124</v>
@@ -3463,10 +3463,10 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>-0.1140692530327002</v>
+        <v>0.1140692530327002</v>
       </c>
       <c r="B43">
-        <v>0.003777014572843958</v>
+        <v>-0.003777014572843958</v>
       </c>
       <c r="C43">
         <v>-0.04494157995906006</v>
@@ -3474,10 +3474,10 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>-0.114672925563359</v>
+        <v>0.114672925563359</v>
       </c>
       <c r="B44">
-        <v>-0.004068177303939098</v>
+        <v>0.004068177303939098</v>
       </c>
       <c r="C44">
         <v>-0.06013259652916059</v>
@@ -3485,10 +3485,10 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>-0.1154931671130773</v>
+        <v>0.1154931671130773</v>
       </c>
       <c r="B45">
-        <v>-0.01183029205118377</v>
+        <v>0.01183029205118377</v>
       </c>
       <c r="C45">
         <v>-0.07484772120854274</v>
@@ -3496,10 +3496,10 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>-0.1165305508495583</v>
+        <v>0.1165305508495583</v>
       </c>
       <c r="B46">
-        <v>-0.01943297374775248</v>
+        <v>0.01943297374775248</v>
       </c>
       <c r="C46">
         <v>-0.08881738572507106</v>
@@ -3507,10 +3507,10 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>-0.1177269485186222</v>
+        <v>0.1177269485186222</v>
       </c>
       <c r="B47">
-        <v>-0.02677774852663677</v>
+        <v>0.02677774852663677</v>
       </c>
       <c r="C47">
         <v>-0.1016883764341552</v>
@@ -3518,10 +3518,10 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>-0.119006967533228</v>
+        <v>0.119006967533228</v>
       </c>
       <c r="B48">
-        <v>-0.03375224609691165</v>
+        <v>0.03375224609691165</v>
       </c>
       <c r="C48">
         <v>-0.1130355815372494</v>
@@ -3529,10 +3529,10 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>-0.1202839163487873</v>
+        <v>0.1202839163487873</v>
       </c>
       <c r="B49">
-        <v>-0.04028312045368849</v>
+        <v>0.04028312045368849</v>
       </c>
       <c r="C49">
         <v>-0.1223924603423906</v>
@@ -3540,10 +3540,10 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>-0.1214556379485759</v>
+        <v>0.1214556379485759</v>
       </c>
       <c r="B50">
-        <v>-0.04631668941238382</v>
+        <v>0.04631668941238382</v>
       </c>
       <c r="C50">
         <v>-0.129313710328427</v>
@@ -3551,10 +3551,10 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>-0.1224057849476866</v>
+        <v>0.1224057849476866</v>
       </c>
       <c r="B51">
-        <v>-0.05182533663358131</v>
+        <v>0.05182533663358131</v>
       </c>
       <c r="C51">
         <v>-0.1334666994811328</v>
@@ -3562,10 +3562,10 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>-0.1230491140443012</v>
+        <v>0.1230491140443012</v>
       </c>
       <c r="B52">
-        <v>-0.05681894029754148</v>
+        <v>0.05681894029754148</v>
       </c>
       <c r="C52">
         <v>-0.1347448387520708</v>
@@ -3573,10 +3573,10 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>-0.1233268227003705</v>
+        <v>0.1233268227003705</v>
       </c>
       <c r="B53">
-        <v>-0.06128894727673403</v>
+        <v>0.06128894727673403</v>
       </c>
       <c r="C53">
         <v>-0.1331586796052998</v>
@@ -3584,10 +3584,10 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>-0.1232366792821226</v>
+        <v>0.1232366792821226</v>
       </c>
       <c r="B54">
-        <v>-0.06523553971000566</v>
+        <v>0.06523553971000566</v>
       </c>
       <c r="C54">
         <v>-0.1287576585669029</v>
@@ -3595,10 +3595,10 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>-0.1228353195153089</v>
+        <v>0.1228353195153089</v>
       </c>
       <c r="B55">
-        <v>-0.06871843866654584</v>
+        <v>0.06871843866654584</v>
       </c>
       <c r="C55">
         <v>-0.1217150605764785</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>-0.1221954001912476</v>
+        <v>0.1221954001912476</v>
       </c>
       <c r="B56">
-        <v>-0.07184939491094641</v>
+        <v>0.07184939491094641</v>
       </c>
       <c r="C56">
         <v>-0.1123102085723662</v>
@@ -3617,10 +3617,10 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>-0.1214031333606612</v>
+        <v>0.1214031333606612</v>
       </c>
       <c r="B57">
-        <v>-0.07470037737350561</v>
+        <v>0.07470037737350561</v>
       </c>
       <c r="C57">
         <v>-0.1008490075047416</v>
@@ -3628,10 +3628,10 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>-0.1205248045267173</v>
+        <v>0.1205248045267173</v>
       </c>
       <c r="B58">
-        <v>-0.07730515374469728</v>
+        <v>0.07730515374469728</v>
       </c>
       <c r="C58">
         <v>-0.08764487787861819</v>
@@ -3639,10 +3639,10 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>-0.1195959071778525</v>
+        <v>0.1195959071778525</v>
       </c>
       <c r="B59">
-        <v>-0.07963545357537179</v>
+        <v>0.07963545357537179</v>
       </c>
       <c r="C59">
         <v>-0.07301412264310475</v>
@@ -3650,10 +3650,10 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>-0.1186613703950178</v>
+        <v>0.1186613703950178</v>
       </c>
       <c r="B60">
-        <v>-0.08160723916976313</v>
+        <v>0.08160723916976313</v>
       </c>
       <c r="C60">
         <v>-0.0572661102574343</v>
@@ -3661,10 +3661,10 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>-0.1177437336621526</v>
+        <v>0.1177437336621526</v>
       </c>
       <c r="B61">
-        <v>-0.08319664562884668</v>
+        <v>0.08319664562884668</v>
       </c>
       <c r="C61">
         <v>-0.04076287030811893</v>
@@ -3672,10 +3672,10 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>-0.1168790803387934</v>
+        <v>0.1168790803387934</v>
       </c>
       <c r="B62">
-        <v>-0.08442267152091852</v>
+        <v>0.08442267152091852</v>
       </c>
       <c r="C62">
         <v>-0.02389231948148374</v>
@@ -3683,10 +3683,10 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>-0.1161240455792814</v>
+        <v>0.1161240455792814</v>
       </c>
       <c r="B63">
-        <v>-0.08533851809013374</v>
+        <v>0.08533851809013374</v>
       </c>
       <c r="C63">
         <v>-0.007013579311433635</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>-0.1155259607977101</v>
+        <v>0.1155259607977101</v>
       </c>
       <c r="B64">
-        <v>-0.0860185640497604</v>
+        <v>0.0860185640497604</v>
       </c>
       <c r="C64">
         <v>0.00953984716844245</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>-0.115108222334808</v>
+        <v>0.115108222334808</v>
       </c>
       <c r="B65">
-        <v>-0.08650878925114763</v>
+        <v>0.08650878925114763</v>
       </c>
       <c r="C65">
         <v>0.02546894761491289</v>
@@ -3716,10 +3716,10 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>-0.1148836371894487</v>
+        <v>0.1148836371894487</v>
       </c>
       <c r="B66">
-        <v>-0.08683576071084344</v>
+        <v>0.08683576071084344</v>
       </c>
       <c r="C66">
         <v>0.04051381324517576</v>
@@ -3727,10 +3727,10 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>-0.1148374077177494</v>
+        <v>0.1148374077177494</v>
       </c>
       <c r="B67">
-        <v>-0.08704661074287627</v>
+        <v>0.08704661074287627</v>
       </c>
       <c r="C67">
         <v>0.05450631767407476</v>
@@ -3738,10 +3738,10 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>-0.114940442365541</v>
+        <v>0.114940442365541</v>
       </c>
       <c r="B68">
-        <v>-0.08719619722812426</v>
+        <v>0.08719619722812426</v>
       </c>
       <c r="C68">
         <v>0.06735808984421601</v>
@@ -3749,10 +3749,10 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>-0.1151877634845399</v>
+        <v>0.1151877634845399</v>
       </c>
       <c r="B69">
-        <v>-0.08733026636333696</v>
+        <v>0.08733026636333696</v>
       </c>
       <c r="C69">
         <v>0.07902022387684671</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>-0.1155446847740357</v>
+        <v>0.1155446847740357</v>
       </c>
       <c r="B70">
-        <v>-0.08747990103078625</v>
+        <v>0.08747990103078625</v>
       </c>
       <c r="C70">
         <v>0.08944570250399832</v>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>-0.1159436866553981</v>
+        <v>0.1159436866553981</v>
       </c>
       <c r="B71">
-        <v>-0.08767923528711384</v>
+        <v>0.08767923528711384</v>
       </c>
       <c r="C71">
         <v>0.09858203572242984</v>
@@ -3782,10 +3782,10 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>-0.1163023727382986</v>
+        <v>0.1163023727382986</v>
       </c>
       <c r="B72">
-        <v>-0.08794912064420639</v>
+        <v>0.08794912064420639</v>
       </c>
       <c r="C72">
         <v>0.1064046634549001</v>
@@ -3793,10 +3793,10 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>-0.1165189832789967</v>
+        <v>0.1165189832789967</v>
       </c>
       <c r="B73">
-        <v>-0.08829840516434319</v>
+        <v>0.08829840516434319</v>
       </c>
       <c r="C73">
         <v>0.1129292581072973</v>
@@ -3804,10 +3804,10 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>-0.1164835223038357</v>
+        <v>0.1164835223038357</v>
       </c>
       <c r="B74">
-        <v>-0.08873402081478829</v>
+        <v>0.08873402081478829</v>
       </c>
       <c r="C74">
         <v>0.1181838707213976</v>
@@ -3815,10 +3815,10 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>-0.1161133585955221</v>
+        <v>0.1161133585955221</v>
       </c>
       <c r="B75">
-        <v>-0.08928742973560602</v>
+        <v>0.08928742973560602</v>
       </c>
       <c r="C75">
         <v>0.1222002304440462</v>
@@ -3826,10 +3826,10 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>-0.1153600326004128</v>
+        <v>0.1153600326004128</v>
       </c>
       <c r="B76">
-        <v>-0.08997515969433463</v>
+        <v>0.08997515969433463</v>
       </c>
       <c r="C76">
         <v>0.1249654630556118</v>
@@ -3837,10 +3837,10 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>-0.1142107508366547</v>
+        <v>0.1142107508366547</v>
       </c>
       <c r="B77">
-        <v>-0.09077937913561625</v>
+        <v>0.09077937913561625</v>
       </c>
       <c r="C77">
         <v>0.1264401806783723</v>
@@ -3848,10 +3848,10 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>-0.1126825682083056</v>
+        <v>0.1126825682083056</v>
       </c>
       <c r="B78">
-        <v>-0.09165682604283548</v>
+        <v>0.09165682604283548</v>
       </c>
       <c r="C78">
         <v>0.1266160259530763</v>
@@ -3859,10 +3859,10 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>-0.1107830033440867</v>
+        <v>0.1107830033440867</v>
       </c>
       <c r="B79">
-        <v>-0.09257780481077689</v>
+        <v>0.09257780481077689</v>
       </c>
       <c r="C79">
         <v>0.125503073832637</v>
@@ -3870,10 +3870,10 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>-0.1085055254543007</v>
+        <v>0.1085055254543007</v>
       </c>
       <c r="B80">
-        <v>-0.09352514736016554</v>
+        <v>0.09352514736016554</v>
       </c>
       <c r="C80">
         <v>0.123111794710043</v>
@@ -3881,10 +3881,10 @@
     </row>
     <row r="81">
       <c r="A81">
-        <v>-0.1058561845378069</v>
+        <v>0.1058561845378069</v>
       </c>
       <c r="B81">
-        <v>-0.094507625677008</v>
+        <v>0.094507625677008</v>
       </c>
       <c r="C81">
         <v>0.1194574380080261</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>-0.1029004326375739</v>
+        <v>0.1029004326375739</v>
       </c>
       <c r="B82">
-        <v>-0.09554210788087959</v>
+        <v>0.09554210788087959</v>
       </c>
       <c r="C82">
         <v>0.114543634239492</v>
@@ -3903,10 +3903,10 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>-0.09972660611048748</v>
+        <v>0.09972660611048748</v>
       </c>
       <c r="B83">
-        <v>-0.09663984972082268</v>
+        <v>0.09663984972082268</v>
       </c>
       <c r="C83">
         <v>0.1083706163286962</v>
@@ -3914,10 +3914,10 @@
     </row>
     <row r="84">
       <c r="A84">
-        <v>-0.09643932545921344</v>
+        <v>0.09643932545921344</v>
       </c>
       <c r="B84">
-        <v>-0.09782868661638794</v>
+        <v>0.09782868661638794</v>
       </c>
       <c r="C84">
         <v>0.1009346676710393</v>
@@ -3925,10 +3925,10 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>-0.09314302800540604</v>
+        <v>0.09314302800540604</v>
       </c>
       <c r="B85">
-        <v>-0.09911508118732211</v>
+        <v>0.09911508118732211</v>
       </c>
       <c r="C85">
         <v>0.09222578621432116</v>
@@ -3936,10 +3936,10 @@
     </row>
     <row r="86">
       <c r="A86">
-        <v>-0.08992726155678313</v>
+        <v>0.08992726155678313</v>
       </c>
       <c r="B86">
-        <v>-0.1004870424996145</v>
+        <v>0.1004870424996145</v>
       </c>
       <c r="C86">
         <v>0.08224025680597859</v>
@@ -3947,10 +3947,10 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>-0.08682759879198783</v>
+        <v>0.08682759879198783</v>
       </c>
       <c r="B87">
-        <v>-0.1019337996773496</v>
+        <v>0.1019337996773496</v>
       </c>
       <c r="C87">
         <v>0.07098458371014446</v>
@@ -3958,10 +3958,10 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>-0.08385223446502425</v>
+        <v>0.08385223446502425</v>
       </c>
       <c r="B88">
-        <v>-0.1034251543065126</v>
+        <v>0.1034251543065126</v>
       </c>
       <c r="C88">
         <v>0.05850556509518146</v>
@@ -3969,10 +3969,10 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>-0.08099213456433688</v>
+        <v>0.08099213456433688</v>
       </c>
       <c r="B89">
-        <v>-0.1049493052078773</v>
+        <v>0.1049493052078773</v>
       </c>
       <c r="C89">
         <v>0.04484646919265599</v>
@@ -3980,10 +3980,10 @@
     </row>
     <row r="90">
       <c r="A90">
-        <v>-0.07821112937253931</v>
+        <v>0.07821112937253931</v>
       </c>
       <c r="B90">
-        <v>-0.1064995318512713</v>
+        <v>0.1064995318512713</v>
       </c>
       <c r="C90">
         <v>0.03002327478951087</v>
@@ -3991,10 +3991,10 @@
     </row>
     <row r="91">
       <c r="A91">
-        <v>-0.07549164029096311</v>
+        <v>0.07549164029096311</v>
       </c>
       <c r="B91">
-        <v>-0.1080406142607434</v>
+        <v>0.1080406142607434</v>
       </c>
       <c r="C91">
         <v>0.0140110757383466</v>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="92">
       <c r="A92">
-        <v>-0.07282729820659282</v>
+        <v>0.07282729820659282</v>
       </c>
       <c r="B92">
-        <v>-0.1095374372967299</v>
+        <v>0.1095374372967299</v>
       </c>
       <c r="C92">
         <v>-0.003168391008868944</v>
@@ -4013,10 +4013,10 @@
     </row>
     <row r="93">
       <c r="A93">
-        <v>-0.07021113095952444</v>
+        <v>0.07021113095952444</v>
       </c>
       <c r="B93">
-        <v>-0.1109647936065532</v>
+        <v>0.1109647936065532</v>
       </c>
       <c r="C93">
         <v>-0.02144803826104346</v>
@@ -4024,10 +4024,10 @@
     </row>
     <row r="94">
       <c r="A94">
-        <v>-0.06762089429452042</v>
+        <v>0.06762089429452042</v>
       </c>
       <c r="B94">
-        <v>-0.112345955457771</v>
+        <v>0.112345955457771</v>
       </c>
       <c r="C94">
         <v>-0.04074270098908049</v>
@@ -4035,10 +4035,10 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>-0.06503739759682531</v>
+        <v>0.06503739759682531</v>
       </c>
       <c r="B95">
-        <v>-0.1137260557441816</v>
+        <v>0.1137260557441816</v>
       </c>
       <c r="C95">
         <v>-0.06090185040425431</v>
@@ -4046,10 +4046,10 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>-0.06243172487795604</v>
+        <v>0.06243172487795604</v>
       </c>
       <c r="B96">
-        <v>-0.1151703019371564</v>
+        <v>0.1151703019371564</v>
       </c>
       <c r="C96">
         <v>-0.08174312895249447</v>
@@ -4057,10 +4057,10 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>-0.0597821937546212</v>
+        <v>0.0597821937546212</v>
       </c>
       <c r="B97">
-        <v>-0.1167258112654936</v>
+        <v>0.1167258112654936</v>
       </c>
       <c r="C97">
         <v>-0.1030926656380046</v>
@@ -4068,10 +4068,10 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>-0.05709641232384591</v>
+        <v>0.05709641232384591</v>
       </c>
       <c r="B98">
-        <v>-0.1184114728822742</v>
+        <v>0.1184114728822742</v>
       </c>
       <c r="C98">
         <v>-0.1247984366025859</v>
@@ -4079,10 +4079,10 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>-0.05439349716927407</v>
+        <v>0.05439349716927407</v>
       </c>
       <c r="B99">
-        <v>-0.120247064547529</v>
+        <v>0.120247064547529</v>
       </c>
       <c r="C99">
         <v>-0.1467528425026699</v>
@@ -4090,10 +4090,10 @@
     </row>
     <row r="100">
       <c r="A100">
-        <v>-0.05169250713897352</v>
+        <v>0.05169250713897352</v>
       </c>
       <c r="B100">
-        <v>-0.1221997950482935</v>
+        <v>0.1221997950482935</v>
       </c>
       <c r="C100">
         <v>-0.1688494854745694</v>
@@ -4101,10 +4101,10 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>-0.04899273549016162</v>
+        <v>0.04899273549016162</v>
       </c>
       <c r="B101">
-        <v>-0.1242072483619488</v>
+        <v>0.1242072483619488</v>
       </c>
       <c r="C101">
         <v>-0.1909998643960533</v>
@@ -4112,10 +4112,10 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>-0.04628588245930788</v>
+        <v>0.04628588245930788</v>
       </c>
       <c r="B102">
-        <v>-0.1262396896588266</v>
+        <v>0.1262396896588266</v>
       </c>
       <c r="C102">
         <v>-0.2131636456649294</v>

</xml_diff>

<commit_message>
remove simresult.zip because it's too big
</commit_message>
<xml_diff>
--- a/figure_table/toyexample_TEMPTED.xlsx
+++ b/figure_table/toyexample_TEMPTED.xlsx
@@ -392,10 +392,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.07880033100398944</v>
+        <v>0.07880033100398944</v>
       </c>
       <c r="C2">
-        <v>0.1214369994391653</v>
+        <v>-0.1214369994391653</v>
       </c>
       <c r="D2">
         <v>0.08286637801416286</v>
@@ -408,10 +408,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.1597047368379094</v>
+        <v>0.1597047368379094</v>
       </c>
       <c r="C3">
-        <v>0.08924064136581804</v>
+        <v>-0.08924064136581804</v>
       </c>
       <c r="D3">
         <v>0.02194583339231184</v>
@@ -424,10 +424,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.09182320861932254</v>
+        <v>0.09182320861932254</v>
       </c>
       <c r="C4">
-        <v>0.1399065702590379</v>
+        <v>-0.1399065702590379</v>
       </c>
       <c r="D4">
         <v>0.08142219514737449</v>
@@ -440,10 +440,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>-0.06885075539748635</v>
+        <v>0.06885075539748635</v>
       </c>
       <c r="C5">
-        <v>0.1507682320556845</v>
+        <v>-0.1507682320556845</v>
       </c>
       <c r="D5">
         <v>0.1828830105495226</v>
@@ -456,10 +456,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.1064637437162154</v>
+        <v>0.1064637437162154</v>
       </c>
       <c r="C6">
-        <v>0.2004787865145692</v>
+        <v>-0.2004787865145692</v>
       </c>
       <c r="D6">
         <v>0.1593372006206886</v>
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>-0.08468212103776607</v>
+        <v>0.08468212103776607</v>
       </c>
       <c r="C7">
-        <v>0.231414938101536</v>
+        <v>-0.231414938101536</v>
       </c>
       <c r="D7">
         <v>0.1374942494335623</v>
@@ -488,10 +488,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>-0.006942093937174086</v>
+        <v>0.006942093937174086</v>
       </c>
       <c r="C8">
-        <v>0.1569134902252004</v>
+        <v>-0.1569134902252004</v>
       </c>
       <c r="D8">
         <v>0.1709881830670296</v>
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>-0.1181267850122958</v>
+        <v>0.1181267850122958</v>
       </c>
       <c r="C9">
-        <v>0.1579221650765876</v>
+        <v>-0.1579221650765876</v>
       </c>
       <c r="D9">
         <v>0.08154890345050997</v>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>-0.03989675258009495</v>
+        <v>0.03989675258009495</v>
       </c>
       <c r="C10">
-        <v>0.149923486753858</v>
+        <v>-0.149923486753858</v>
       </c>
       <c r="D10">
         <v>0.181058889512264</v>
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.03398321206824673</v>
+        <v>0.03398321206824673</v>
       </c>
       <c r="C11">
-        <v>0.1325572000438724</v>
+        <v>-0.1325572000438724</v>
       </c>
       <c r="D11">
         <v>0.09324971122061536</v>
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B12">
-        <v>-0.0393834362513036</v>
+        <v>0.0393834362513036</v>
       </c>
       <c r="C12">
-        <v>0.1069070723376464</v>
+        <v>-0.1069070723376464</v>
       </c>
       <c r="D12">
         <v>0.06029063684868469</v>
@@ -568,10 +568,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>-0.06418415895501667</v>
+        <v>0.06418415895501667</v>
       </c>
       <c r="C13">
-        <v>0.1279859881148709</v>
+        <v>-0.1279859881148709</v>
       </c>
       <c r="D13">
         <v>0.1195667273895422</v>
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>-0.07242971303684753</v>
+        <v>0.07242971303684753</v>
       </c>
       <c r="C14">
-        <v>0.1494128835333963</v>
+        <v>-0.1494128835333963</v>
       </c>
       <c r="D14">
         <v>0.04266706133200412</v>
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>-0.09029877826118225</v>
+        <v>0.09029877826118225</v>
       </c>
       <c r="C15">
-        <v>0.1625674025572098</v>
+        <v>-0.1625674025572098</v>
       </c>
       <c r="D15">
         <v>0.05610808754397775</v>
@@ -616,10 +616,10 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.0326595669318467</v>
+        <v>0.0326595669318467</v>
       </c>
       <c r="C16">
-        <v>0.1491304409524304</v>
+        <v>-0.1491304409524304</v>
       </c>
       <c r="D16">
         <v>0.08068434163336682</v>
@@ -632,10 +632,10 @@
         </is>
       </c>
       <c r="B17">
-        <v>-0.05572218326875031</v>
+        <v>0.05572218326875031</v>
       </c>
       <c r="C17">
-        <v>0.1282802804216011</v>
+        <v>-0.1282802804216011</v>
       </c>
       <c r="D17">
         <v>0.06982946815661424</v>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B18">
-        <v>-0.1188887401453342</v>
+        <v>0.1188887401453342</v>
       </c>
       <c r="C18">
-        <v>0.196080812070059</v>
+        <v>-0.196080812070059</v>
       </c>
       <c r="D18">
         <v>0.08348757761444664</v>
@@ -664,10 +664,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>-0.09593907800657581</v>
+        <v>0.09593907800657581</v>
       </c>
       <c r="C19">
-        <v>0.1112069989509569</v>
+        <v>-0.1112069989509569</v>
       </c>
       <c r="D19">
         <v>0.2161882178419718</v>
@@ -680,10 +680,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>-0.059080270576451</v>
+        <v>0.059080270576451</v>
       </c>
       <c r="C20">
-        <v>0.1287622198577844</v>
+        <v>-0.1287622198577844</v>
       </c>
       <c r="D20">
         <v>0.06929104037800883</v>
@@ -696,10 +696,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>-0.1086246116494793</v>
+        <v>0.1086246116494793</v>
       </c>
       <c r="C21">
-        <v>0.2478063645090004</v>
+        <v>-0.2478063645090004</v>
       </c>
       <c r="D21">
         <v>0.1040687696044373</v>
@@ -712,10 +712,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>-0.1207840450460627</v>
+        <v>0.1207840450460627</v>
       </c>
       <c r="C22">
-        <v>0.0400602660338118</v>
+        <v>-0.0400602660338118</v>
       </c>
       <c r="D22">
         <v>0.1523271192084657</v>
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>-0.1424967482471836</v>
+        <v>0.1424967482471836</v>
       </c>
       <c r="C23">
-        <v>-0.04804290026338388</v>
+        <v>0.04804290026338388</v>
       </c>
       <c r="D23">
         <v>0.1215239350647906</v>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B24">
-        <v>-0.1841318024115703</v>
+        <v>0.1841318024115703</v>
       </c>
       <c r="C24">
-        <v>0.05304303404014515</v>
+        <v>-0.05304303404014515</v>
       </c>
       <c r="D24">
         <v>0.1052458977956333</v>
@@ -760,10 +760,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>-0.1880883407097291</v>
+        <v>0.1880883407097291</v>
       </c>
       <c r="C25">
-        <v>0.04652472903038417</v>
+        <v>-0.04652472903038417</v>
       </c>
       <c r="D25">
         <v>0.07786685759590449</v>
@@ -776,10 +776,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.1166535035664137</v>
+        <v>0.1166535035664137</v>
       </c>
       <c r="C26">
-        <v>0.05331014115494709</v>
+        <v>-0.05331014115494709</v>
       </c>
       <c r="D26">
         <v>0.1084221622006323</v>
@@ -792,10 +792,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>-0.1489222249139132</v>
+        <v>0.1489222249139132</v>
       </c>
       <c r="C27">
-        <v>0.01787104103422705</v>
+        <v>-0.01787104103422705</v>
       </c>
       <c r="D27">
         <v>0.1304433213087429</v>
@@ -808,10 +808,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>-0.1361027041258603</v>
+        <v>0.1361027041258603</v>
       </c>
       <c r="C28">
-        <v>-0.04405263595672025</v>
+        <v>0.04405263595672025</v>
       </c>
       <c r="D28">
         <v>0.1052854343647315</v>
@@ -824,10 +824,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>-0.1246603111788643</v>
+        <v>0.1246603111788643</v>
       </c>
       <c r="C29">
-        <v>-0.004160658796581899</v>
+        <v>0.004160658796581899</v>
       </c>
       <c r="D29">
         <v>0.09807544077649784</v>
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>-0.1574420473153161</v>
+        <v>0.1574420473153161</v>
       </c>
       <c r="C30">
-        <v>0.06313717410600292</v>
+        <v>-0.06313717410600292</v>
       </c>
       <c r="D30">
         <v>0.1041393907348075</v>
@@ -856,10 +856,10 @@
         </is>
       </c>
       <c r="B31">
-        <v>-0.1060189038618903</v>
+        <v>0.1060189038618903</v>
       </c>
       <c r="C31">
-        <v>0.08657780365855253</v>
+        <v>-0.08657780365855253</v>
       </c>
       <c r="D31">
         <v>0.04694756544500957</v>
@@ -872,10 +872,10 @@
         </is>
       </c>
       <c r="B32">
-        <v>-0.1568412589673558</v>
+        <v>0.1568412589673558</v>
       </c>
       <c r="C32">
-        <v>-0.0087038431122955</v>
+        <v>0.0087038431122955</v>
       </c>
       <c r="D32">
         <v>0.09739018354220523</v>
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>-0.1518207445508232</v>
+        <v>0.1518207445508232</v>
       </c>
       <c r="C33">
-        <v>0.01938041579834017</v>
+        <v>-0.01938041579834017</v>
       </c>
       <c r="D33">
         <v>0.1035820134209568</v>
@@ -904,10 +904,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>-0.08476183168910413</v>
+        <v>0.08476183168910413</v>
       </c>
       <c r="C34">
-        <v>-0.0488533308951106</v>
+        <v>0.0488533308951106</v>
       </c>
       <c r="D34">
         <v>0.09051974234979543</v>
@@ -920,10 +920,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>-0.1904791751848131</v>
+        <v>0.1904791751848131</v>
       </c>
       <c r="C35">
-        <v>-0.006666381894677296</v>
+        <v>0.006666381894677296</v>
       </c>
       <c r="D35">
         <v>0.1115794817294884</v>
@@ -936,10 +936,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>-0.1197296066625953</v>
+        <v>0.1197296066625953</v>
       </c>
       <c r="C36">
-        <v>-0.04137040799836017</v>
+        <v>0.04137040799836017</v>
       </c>
       <c r="D36">
         <v>0.191588624992434</v>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>-0.09845232729245383</v>
+        <v>0.09845232729245383</v>
       </c>
       <c r="C37">
-        <v>0.02353201588609518</v>
+        <v>-0.02353201588609518</v>
       </c>
       <c r="D37">
         <v>0.2011007193876927</v>
@@ -968,10 +968,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>-0.1504012091219676</v>
+        <v>0.1504012091219676</v>
       </c>
       <c r="C38">
-        <v>-0.02765697563870612</v>
+        <v>0.02765697563870612</v>
       </c>
       <c r="D38">
         <v>0.100213658553973</v>
@@ -984,10 +984,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>-0.07122830914109726</v>
+        <v>0.07122830914109726</v>
       </c>
       <c r="C39">
-        <v>0.07506640441448975</v>
+        <v>-0.07506640441448975</v>
       </c>
       <c r="D39">
         <v>0.2206316210571686</v>
@@ -1000,10 +1000,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>-0.2265197967315946</v>
+        <v>0.2265197967315946</v>
       </c>
       <c r="C40">
-        <v>-0.04740057954479043</v>
+        <v>0.04740057954479043</v>
       </c>
       <c r="D40">
         <v>0.01361621534738438</v>
@@ -1016,10 +1016,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>-0.1613174140009147</v>
+        <v>0.1613174140009147</v>
       </c>
       <c r="C41">
-        <v>-0.009525502976460364</v>
+        <v>0.009525502976460364</v>
       </c>
       <c r="D41">
         <v>0.1016482954363994</v>
@@ -1032,10 +1032,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.1524815940947832</v>
+        <v>-0.1524815940947832</v>
       </c>
       <c r="C42">
-        <v>0.09539351800340515</v>
+        <v>-0.09539351800340515</v>
       </c>
       <c r="D42">
         <v>0.07907566791150117</v>
@@ -1048,10 +1048,10 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.1006952260212896</v>
+        <v>-0.1006952260212896</v>
       </c>
       <c r="C43">
-        <v>0.1754087969904064</v>
+        <v>-0.1754087969904064</v>
       </c>
       <c r="D43">
         <v>0.1010814514830914</v>
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.1297706116613269</v>
+        <v>-0.1297706116613269</v>
       </c>
       <c r="C44">
-        <v>0.16258805335235</v>
+        <v>-0.16258805335235</v>
       </c>
       <c r="D44">
         <v>0.1126153295510959</v>
@@ -1080,10 +1080,10 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.06887893405855348</v>
+        <v>-0.06887893405855348</v>
       </c>
       <c r="C45">
-        <v>0.2011623620254935</v>
+        <v>-0.2011623620254935</v>
       </c>
       <c r="D45">
         <v>0.1052471457489279</v>
@@ -1096,10 +1096,10 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.1286975011557017</v>
+        <v>-0.1286975011557017</v>
       </c>
       <c r="C46">
-        <v>0.1366386636569925</v>
+        <v>-0.1366386636569925</v>
       </c>
       <c r="D46">
         <v>0.1089611643971406</v>
@@ -1112,10 +1112,10 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.1391387690211929</v>
+        <v>-0.1391387690211929</v>
       </c>
       <c r="C47">
-        <v>0.1430096268577066</v>
+        <v>-0.1430096268577066</v>
       </c>
       <c r="D47">
         <v>0.1007542559006574</v>
@@ -1128,10 +1128,10 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.08871823613264167</v>
+        <v>-0.08871823613264167</v>
       </c>
       <c r="C48">
-        <v>0.2535098651157587</v>
+        <v>-0.2535098651157587</v>
       </c>
       <c r="D48">
         <v>0.1150785997162549</v>
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.1877606920033705</v>
+        <v>-0.1877606920033705</v>
       </c>
       <c r="C49">
-        <v>0.1148520871673355</v>
+        <v>-0.1148520871673355</v>
       </c>
       <c r="D49">
         <v>0.201843583806864</v>
@@ -1160,10 +1160,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.1569417085128846</v>
+        <v>-0.1569417085128846</v>
       </c>
       <c r="C50">
-        <v>0.1367260694464659</v>
+        <v>-0.1367260694464659</v>
       </c>
       <c r="D50">
         <v>0.2812543447786442</v>
@@ -1176,10 +1176,10 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.1594157473842039</v>
+        <v>-0.1594157473842039</v>
       </c>
       <c r="C51">
-        <v>0.126431634358593</v>
+        <v>-0.126431634358593</v>
       </c>
       <c r="D51">
         <v>0.222429672884922</v>
@@ -1192,10 +1192,10 @@
         </is>
       </c>
       <c r="B52">
-        <v>0.166420343368233</v>
+        <v>-0.166420343368233</v>
       </c>
       <c r="C52">
-        <v>0.1029979520168319</v>
+        <v>-0.1029979520168319</v>
       </c>
       <c r="D52">
         <v>0.1730408711989471</v>
@@ -1208,10 +1208,10 @@
         </is>
       </c>
       <c r="B53">
-        <v>0.1389604624739776</v>
+        <v>-0.1389604624739776</v>
       </c>
       <c r="C53">
-        <v>0.07987778110635416</v>
+        <v>-0.07987778110635416</v>
       </c>
       <c r="D53">
         <v>0.07531211867155593</v>
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B54">
-        <v>0.09480884968176284</v>
+        <v>-0.09480884968176284</v>
       </c>
       <c r="C54">
-        <v>0.136970448380681</v>
+        <v>-0.136970448380681</v>
       </c>
       <c r="D54">
         <v>0.1058745716315293</v>
@@ -1240,10 +1240,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>0.171837564703721</v>
+        <v>-0.171837564703721</v>
       </c>
       <c r="C55">
-        <v>0.1385598712777725</v>
+        <v>-0.1385598712777725</v>
       </c>
       <c r="D55">
         <v>0.1060105896373873</v>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>0.192171193283747</v>
+        <v>-0.192171193283747</v>
       </c>
       <c r="C56">
-        <v>0.1387569041945457</v>
+        <v>-0.1387569041945457</v>
       </c>
       <c r="D56">
         <v>0.1729712366942464</v>
@@ -1272,10 +1272,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>0.2048876041419146</v>
+        <v>-0.2048876041419146</v>
       </c>
       <c r="C57">
-        <v>0.08165555404799489</v>
+        <v>-0.08165555404799489</v>
       </c>
       <c r="D57">
         <v>0.1692860454501073</v>
@@ -1288,10 +1288,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>0.1636535110991047</v>
+        <v>-0.1636535110991047</v>
       </c>
       <c r="C58">
-        <v>0.1410792001829381</v>
+        <v>-0.1410792001829381</v>
       </c>
       <c r="D58">
         <v>0.1310094319869677</v>
@@ -1304,10 +1304,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>0.09529976887725825</v>
+        <v>-0.09529976887725825</v>
       </c>
       <c r="C59">
-        <v>0.1489229712502358</v>
+        <v>-0.1489229712502358</v>
       </c>
       <c r="D59">
         <v>0.08593932294132844</v>
@@ -1320,10 +1320,10 @@
         </is>
       </c>
       <c r="B60">
-        <v>0.1704178216584816</v>
+        <v>-0.1704178216584816</v>
       </c>
       <c r="C60">
-        <v>0.1004813114613144</v>
+        <v>-0.1004813114613144</v>
       </c>
       <c r="D60">
         <v>0.09599681296790769</v>
@@ -1336,10 +1336,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>0.1198211957719144</v>
+        <v>-0.1198211957719144</v>
       </c>
       <c r="C61">
-        <v>0.277698010227947</v>
+        <v>-0.277698010227947</v>
       </c>
       <c r="D61">
         <v>0.1649019368160083</v>
@@ -3012,10 +3012,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0.03584611425551176</v>
+        <v>-0.03584611425551176</v>
       </c>
       <c r="B2">
-        <v>-0.1261660229675725</v>
+        <v>0.1261660229675725</v>
       </c>
       <c r="C2">
         <v>-0.2114090648450627</v>
@@ -3023,10 +3023,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.03888348454188601</v>
+        <v>-0.03888348454188601</v>
       </c>
       <c r="B3">
-        <v>-0.1280966100874439</v>
+        <v>0.1280966100874439</v>
       </c>
       <c r="C3">
         <v>-0.1908208461452241</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.04190078771077085</v>
+        <v>-0.04190078771077085</v>
       </c>
       <c r="B4">
-        <v>-0.1300479773889831</v>
+        <v>0.1300479773889831</v>
       </c>
       <c r="C4">
         <v>-0.1702523380531559</v>
@@ -3045,10 +3045,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.04485766930607214</v>
+        <v>-0.04485766930607214</v>
       </c>
       <c r="B5">
-        <v>-0.1320303666728868</v>
+        <v>0.1320303666728868</v>
       </c>
       <c r="C5">
         <v>-0.1497399351875364</v>
@@ -3056,10 +3056,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.04771968755473609</v>
+        <v>-0.04771968755473609</v>
       </c>
       <c r="B6">
-        <v>-0.1340030946923663</v>
+        <v>0.1340030946923663</v>
       </c>
       <c r="C6">
         <v>-0.1293541106290052</v>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.05049449189690745</v>
+        <v>-0.05049449189690745</v>
       </c>
       <c r="B7">
-        <v>-0.1358767400937768</v>
+        <v>0.1358767400937768</v>
       </c>
       <c r="C7">
         <v>-0.1091667532894945</v>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.05323720007498162</v>
+        <v>-0.05323720007498162</v>
       </c>
       <c r="B8">
-        <v>-0.1375873429855182</v>
+        <v>0.1375873429855182</v>
       </c>
       <c r="C8">
         <v>-0.08923731780255828</v>
@@ -3089,10 +3089,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.05602764123582211</v>
+        <v>-0.05602764123582211</v>
       </c>
       <c r="B9">
-        <v>-0.139112344381051</v>
+        <v>0.139112344381051</v>
       </c>
       <c r="C9">
         <v>-0.06960621210965814</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.05891856211600118</v>
+        <v>-0.05891856211600118</v>
       </c>
       <c r="B10">
-        <v>-0.1403709563575088</v>
+        <v>0.1403709563575088</v>
       </c>
       <c r="C10">
         <v>-0.05037354421408783</v>
@@ -3111,10 +3111,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.06192080305161932</v>
+        <v>-0.06192080305161932</v>
       </c>
       <c r="B11">
-        <v>-0.1412620094606763</v>
+        <v>0.1412620094606763</v>
       </c>
       <c r="C11">
         <v>-0.03166623998205532</v>
@@ -3122,10 +3122,10 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>0.06502997221068191</v>
+        <v>-0.06502997221068191</v>
       </c>
       <c r="B12">
-        <v>-0.1417049914353085</v>
+        <v>0.1417049914353085</v>
       </c>
       <c r="C12">
         <v>-0.0136124037126967</v>
@@ -3133,10 +3133,10 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>0.0682217927374613</v>
+        <v>-0.0682217927374613</v>
       </c>
       <c r="B13">
-        <v>-0.1417017789286655</v>
+        <v>0.1417017789286655</v>
       </c>
       <c r="C13">
         <v>0.003655262130591408</v>
@@ -3144,10 +3144,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>0.07147981864187419</v>
+        <v>-0.07147981864187419</v>
       </c>
       <c r="B14">
-        <v>-0.1412829067322424</v>
+        <v>0.1412829067322424</v>
       </c>
       <c r="C14">
         <v>0.02002067260579577</v>
@@ -3155,10 +3155,10 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>0.07479378898660065</v>
+        <v>-0.07479378898660065</v>
       </c>
       <c r="B15">
-        <v>-0.1404766937034764</v>
+        <v>0.1404766937034764</v>
       </c>
       <c r="C15">
         <v>0.03541008150476255</v>
@@ -3166,10 +3166,10 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>0.07813776785780477</v>
+        <v>-0.07813776785780477</v>
       </c>
       <c r="B16">
-        <v>-0.1393327134303599</v>
+        <v>0.1393327134303599</v>
       </c>
       <c r="C16">
         <v>0.04973524646842393</v>
@@ -3177,10 +3177,10 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>0.0814609933235251</v>
+        <v>-0.0814609933235251</v>
       </c>
       <c r="B17">
-        <v>-0.1379115473026885</v>
+        <v>0.1379115473026885</v>
       </c>
       <c r="C17">
         <v>0.06291090653511749</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>0.0847460889320646</v>
+        <v>-0.0847460889320646</v>
       </c>
       <c r="B18">
-        <v>-0.1362359448069206</v>
+        <v>0.1362359448069206</v>
       </c>
       <c r="C18">
         <v>0.07489361441684624</v>
@@ -3199,10 +3199,10 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>0.08798957340369122</v>
+        <v>-0.08798957340369122</v>
       </c>
       <c r="B19">
-        <v>-0.13431261277634</v>
+        <v>0.13431261277634</v>
       </c>
       <c r="C19">
         <v>0.08567338841457367</v>
@@ -3210,10 +3210,10 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>0.09116892161060079</v>
+        <v>-0.09116892161060079</v>
       </c>
       <c r="B20">
-        <v>-0.1321639880710429</v>
+        <v>0.1321639880710429</v>
       </c>
       <c r="C20">
         <v>0.0952191600999244</v>
@@ -3221,10 +3221,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>0.09425152007691803</v>
+        <v>-0.09425152007691803</v>
       </c>
       <c r="B21">
-        <v>-0.129792202374663</v>
+        <v>0.129792202374663</v>
       </c>
       <c r="C21">
         <v>0.1034293501194486</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>0.09718356612790389</v>
+        <v>-0.09718356612790389</v>
       </c>
       <c r="B22">
-        <v>-0.1271917421652431</v>
+        <v>0.1271917421652431</v>
       </c>
       <c r="C22">
         <v>0.1101934723703826</v>
@@ -3243,10 +3243,10 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>0.0999147371795141</v>
+        <v>-0.0999147371795141</v>
       </c>
       <c r="B23">
-        <v>-0.1243474336847771</v>
+        <v>0.1243474336847771</v>
       </c>
       <c r="C23">
         <v>0.1154325310850253</v>
@@ -3254,10 +3254,10 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>0.1024411458943892</v>
+        <v>-0.1024411458943892</v>
       </c>
       <c r="B24">
-        <v>-0.1212491236992373</v>
+        <v>0.1212491236992373</v>
       </c>
       <c r="C24">
         <v>0.1191109387747327</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.104758855565474</v>
+        <v>-0.104758855565474</v>
       </c>
       <c r="B25">
-        <v>-0.1178570458575076</v>
+        <v>0.1178570458575076</v>
       </c>
       <c r="C25">
         <v>0.121241093243928</v>
@@ -3276,10 +3276,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>0.1068821113627917</v>
+        <v>-0.1068821113627917</v>
       </c>
       <c r="B26">
-        <v>-0.1141234166013049</v>
+        <v>0.1141234166013049</v>
       </c>
       <c r="C26">
         <v>0.1218533141761865</v>
@@ -3287,10 +3287,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>0.1088122123022573</v>
+        <v>-0.1088122123022573</v>
       </c>
       <c r="B27">
-        <v>-0.1100091261522422</v>
+        <v>0.1100091261522422</v>
       </c>
       <c r="C27">
         <v>0.1210042011080165</v>
@@ -3298,10 +3298,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>0.1104941612425646</v>
+        <v>-0.1104941612425646</v>
       </c>
       <c r="B28">
-        <v>-0.1054996126930566</v>
+        <v>0.1054996126930566</v>
       </c>
       <c r="C28">
         <v>0.1187307541634631</v>
@@ -3309,10 +3309,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>0.1118783610632255</v>
+        <v>-0.1118783610632255</v>
       </c>
       <c r="B29">
-        <v>-0.1006290414523116</v>
+        <v>0.1006290414523116</v>
       </c>
       <c r="C29">
         <v>0.1150658859673596</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>0.1129648114253242</v>
+        <v>-0.1129648114253242</v>
       </c>
       <c r="B30">
-        <v>-0.09542311040749513</v>
+        <v>0.09542311040749513</v>
       </c>
       <c r="C30">
         <v>0.1100693033274244</v>
@@ -3331,10 +3331,10 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>0.1137631319739484</v>
+        <v>-0.1137631319739484</v>
       </c>
       <c r="B31">
-        <v>-0.0898902283505609</v>
+        <v>0.0898902283505609</v>
       </c>
       <c r="C31">
         <v>0.1038190413265975</v>
@@ -3342,10 +3342,10 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>0.1142600113166586</v>
+        <v>-0.1142600113166586</v>
       </c>
       <c r="B32">
-        <v>-0.08402796676416481</v>
+        <v>0.08402796676416481</v>
       </c>
       <c r="C32">
         <v>0.09636623408259679</v>
@@ -3353,10 +3353,10 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>0.1144563690838302</v>
+        <v>-0.1144563690838302</v>
       </c>
       <c r="B33">
-        <v>-0.07785485117788461</v>
+        <v>0.07785485117788461</v>
       </c>
       <c r="C33">
         <v>0.08777310153522087</v>
@@ -3364,10 +3364,10 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>0.1144043171831065</v>
+        <v>-0.1144043171831065</v>
       </c>
       <c r="B34">
-        <v>-0.07138520866556547</v>
+        <v>0.07138520866556547</v>
       </c>
       <c r="C34">
         <v>0.07810488671683126</v>
@@ -3375,10 +3375,10 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>0.1142021332788516</v>
+        <v>-0.1142021332788516</v>
       </c>
       <c r="B35">
-        <v>-0.06460178118966367</v>
+        <v>0.06460178118966367</v>
       </c>
       <c r="C35">
         <v>0.067394993701182</v>
@@ -3386,10 +3386,10 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>0.1139490195579526</v>
+        <v>-0.1139490195579526</v>
       </c>
       <c r="B36">
-        <v>-0.05753619880781555</v>
+        <v>0.05753619880781555</v>
       </c>
       <c r="C36">
         <v>0.05569652325763148</v>
@@ -3397,10 +3397,10 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>0.1137118752692501</v>
+        <v>-0.1137118752692501</v>
       </c>
       <c r="B37">
-        <v>-0.05024153762267213</v>
+        <v>0.05024153762267213</v>
       </c>
       <c r="C37">
         <v>0.04310554140968866</v>
@@ -3408,10 +3408,10 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>0.1135261950400183</v>
+        <v>-0.1135261950400183</v>
       </c>
       <c r="B38">
-        <v>-0.0427547203437779</v>
+        <v>0.0427547203437779</v>
       </c>
       <c r="C38">
         <v>0.02972379916907733</v>
@@ -3419,10 +3419,10 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>0.1133952595789638</v>
+        <v>-0.1133952595789638</v>
       </c>
       <c r="B39">
-        <v>-0.03510418176991831</v>
+        <v>0.03510418176991831</v>
       </c>
       <c r="C39">
         <v>0.01564281432055305</v>
@@ -3430,10 +3430,10 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>0.1133439230422368</v>
+        <v>-0.1133439230422368</v>
       </c>
       <c r="B40">
-        <v>-0.02734071614690875</v>
+        <v>0.02734071614690875</v>
       </c>
       <c r="C40">
         <v>0.0009725763272283479</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>0.1134246352605632</v>
+        <v>-0.1134246352605632</v>
       </c>
       <c r="B41">
-        <v>-0.01951218510840367</v>
+        <v>0.01951218510840367</v>
       </c>
       <c r="C41">
         <v>-0.01414504278215793</v>
@@ -3452,10 +3452,10 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>0.1136633701498238</v>
+        <v>-0.1136633701498238</v>
       </c>
       <c r="B42">
-        <v>-0.01164778875484332</v>
+        <v>0.01164778875484332</v>
       </c>
       <c r="C42">
         <v>-0.02952782495901124</v>
@@ -3463,10 +3463,10 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>0.1140692530327002</v>
+        <v>-0.1140692530327002</v>
       </c>
       <c r="B43">
-        <v>-0.003777014572843958</v>
+        <v>0.003777014572843958</v>
       </c>
       <c r="C43">
         <v>-0.04494157995906006</v>
@@ -3474,10 +3474,10 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>0.114672925563359</v>
+        <v>-0.114672925563359</v>
       </c>
       <c r="B44">
-        <v>0.004068177303939098</v>
+        <v>-0.004068177303939098</v>
       </c>
       <c r="C44">
         <v>-0.06013259652916059</v>
@@ -3485,10 +3485,10 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>0.1154931671130773</v>
+        <v>-0.1154931671130773</v>
       </c>
       <c r="B45">
-        <v>0.01183029205118377</v>
+        <v>-0.01183029205118377</v>
       </c>
       <c r="C45">
         <v>-0.07484772120854274</v>
@@ -3496,10 +3496,10 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>0.1165305508495583</v>
+        <v>-0.1165305508495583</v>
       </c>
       <c r="B46">
-        <v>0.01943297374775248</v>
+        <v>-0.01943297374775248</v>
       </c>
       <c r="C46">
         <v>-0.08881738572507106</v>
@@ -3507,10 +3507,10 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>0.1177269485186222</v>
+        <v>-0.1177269485186222</v>
       </c>
       <c r="B47">
-        <v>0.02677774852663677</v>
+        <v>-0.02677774852663677</v>
       </c>
       <c r="C47">
         <v>-0.1016883764341552</v>
@@ -3518,10 +3518,10 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>0.119006967533228</v>
+        <v>-0.119006967533228</v>
       </c>
       <c r="B48">
-        <v>0.03375224609691165</v>
+        <v>-0.03375224609691165</v>
       </c>
       <c r="C48">
         <v>-0.1130355815372494</v>
@@ -3529,10 +3529,10 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>0.1202839163487873</v>
+        <v>-0.1202839163487873</v>
       </c>
       <c r="B49">
-        <v>0.04028312045368849</v>
+        <v>-0.04028312045368849</v>
       </c>
       <c r="C49">
         <v>-0.1223924603423906</v>
@@ -3540,10 +3540,10 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>0.1214556379485759</v>
+        <v>-0.1214556379485759</v>
       </c>
       <c r="B50">
-        <v>0.04631668941238382</v>
+        <v>-0.04631668941238382</v>
       </c>
       <c r="C50">
         <v>-0.129313710328427</v>
@@ -3551,10 +3551,10 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>0.1224057849476866</v>
+        <v>-0.1224057849476866</v>
       </c>
       <c r="B51">
-        <v>0.05182533663358131</v>
+        <v>-0.05182533663358131</v>
       </c>
       <c r="C51">
         <v>-0.1334666994811328</v>
@@ -3562,10 +3562,10 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>0.1230491140443012</v>
+        <v>-0.1230491140443012</v>
       </c>
       <c r="B52">
-        <v>0.05681894029754148</v>
+        <v>-0.05681894029754148</v>
       </c>
       <c r="C52">
         <v>-0.1347448387520708</v>
@@ -3573,10 +3573,10 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>0.1233268227003705</v>
+        <v>-0.1233268227003705</v>
       </c>
       <c r="B53">
-        <v>0.06128894727673403</v>
+        <v>-0.06128894727673403</v>
       </c>
       <c r="C53">
         <v>-0.1331586796052998</v>
@@ -3584,10 +3584,10 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>0.1232366792821226</v>
+        <v>-0.1232366792821226</v>
       </c>
       <c r="B54">
-        <v>0.06523553971000566</v>
+        <v>-0.06523553971000566</v>
       </c>
       <c r="C54">
         <v>-0.1287576585669029</v>
@@ -3595,10 +3595,10 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>0.1228353195153089</v>
+        <v>-0.1228353195153089</v>
       </c>
       <c r="B55">
-        <v>0.06871843866654584</v>
+        <v>-0.06871843866654584</v>
       </c>
       <c r="C55">
         <v>-0.1217150605764785</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>0.1221954001912476</v>
+        <v>-0.1221954001912476</v>
       </c>
       <c r="B56">
-        <v>0.07184939491094641</v>
+        <v>-0.07184939491094641</v>
       </c>
       <c r="C56">
         <v>-0.1123102085723662</v>
@@ -3617,10 +3617,10 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>0.1214031333606612</v>
+        <v>-0.1214031333606612</v>
       </c>
       <c r="B57">
-        <v>0.07470037737350561</v>
+        <v>-0.07470037737350561</v>
       </c>
       <c r="C57">
         <v>-0.1008490075047416</v>
@@ -3628,10 +3628,10 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>0.1205248045267173</v>
+        <v>-0.1205248045267173</v>
       </c>
       <c r="B58">
-        <v>0.07730515374469728</v>
+        <v>-0.07730515374469728</v>
       </c>
       <c r="C58">
         <v>-0.08764487787861819</v>
@@ -3639,10 +3639,10 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>0.1195959071778525</v>
+        <v>-0.1195959071778525</v>
       </c>
       <c r="B59">
-        <v>0.07963545357537179</v>
+        <v>-0.07963545357537179</v>
       </c>
       <c r="C59">
         <v>-0.07301412264310475</v>
@@ -3650,10 +3650,10 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>0.1186613703950178</v>
+        <v>-0.1186613703950178</v>
       </c>
       <c r="B60">
-        <v>0.08160723916976313</v>
+        <v>-0.08160723916976313</v>
       </c>
       <c r="C60">
         <v>-0.0572661102574343</v>
@@ -3661,10 +3661,10 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>0.1177437336621526</v>
+        <v>-0.1177437336621526</v>
       </c>
       <c r="B61">
-        <v>0.08319664562884668</v>
+        <v>-0.08319664562884668</v>
       </c>
       <c r="C61">
         <v>-0.04076287030811893</v>
@@ -3672,10 +3672,10 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>0.1168790803387934</v>
+        <v>-0.1168790803387934</v>
       </c>
       <c r="B62">
-        <v>0.08442267152091852</v>
+        <v>-0.08442267152091852</v>
       </c>
       <c r="C62">
         <v>-0.02389231948148374</v>
@@ -3683,10 +3683,10 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>0.1161240455792814</v>
+        <v>-0.1161240455792814</v>
       </c>
       <c r="B63">
-        <v>0.08533851809013374</v>
+        <v>-0.08533851809013374</v>
       </c>
       <c r="C63">
         <v>-0.007013579311433635</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>0.1155259607977101</v>
+        <v>-0.1155259607977101</v>
       </c>
       <c r="B64">
-        <v>0.0860185640497604</v>
+        <v>-0.0860185640497604</v>
       </c>
       <c r="C64">
         <v>0.00953984716844245</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>0.115108222334808</v>
+        <v>-0.115108222334808</v>
       </c>
       <c r="B65">
-        <v>0.08650878925114763</v>
+        <v>-0.08650878925114763</v>
       </c>
       <c r="C65">
         <v>0.02546894761491289</v>
@@ -3716,10 +3716,10 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>0.1148836371894487</v>
+        <v>-0.1148836371894487</v>
       </c>
       <c r="B66">
-        <v>0.08683576071084344</v>
+        <v>-0.08683576071084344</v>
       </c>
       <c r="C66">
         <v>0.04051381324517576</v>
@@ -3727,10 +3727,10 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>0.1148374077177494</v>
+        <v>-0.1148374077177494</v>
       </c>
       <c r="B67">
-        <v>0.08704661074287627</v>
+        <v>-0.08704661074287627</v>
       </c>
       <c r="C67">
         <v>0.05450631767407476</v>
@@ -3738,10 +3738,10 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>0.114940442365541</v>
+        <v>-0.114940442365541</v>
       </c>
       <c r="B68">
-        <v>0.08719619722812426</v>
+        <v>-0.08719619722812426</v>
       </c>
       <c r="C68">
         <v>0.06735808984421601</v>
@@ -3749,10 +3749,10 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>0.1151877634845399</v>
+        <v>-0.1151877634845399</v>
       </c>
       <c r="B69">
-        <v>0.08733026636333696</v>
+        <v>-0.08733026636333696</v>
       </c>
       <c r="C69">
         <v>0.07902022387684671</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>0.1155446847740357</v>
+        <v>-0.1155446847740357</v>
       </c>
       <c r="B70">
-        <v>0.08747990103078625</v>
+        <v>-0.08747990103078625</v>
       </c>
       <c r="C70">
         <v>0.08944570250399832</v>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>0.1159436866553981</v>
+        <v>-0.1159436866553981</v>
       </c>
       <c r="B71">
-        <v>0.08767923528711384</v>
+        <v>-0.08767923528711384</v>
       </c>
       <c r="C71">
         <v>0.09858203572242984</v>
@@ -3782,10 +3782,10 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>0.1163023727382986</v>
+        <v>-0.1163023727382986</v>
       </c>
       <c r="B72">
-        <v>0.08794912064420639</v>
+        <v>-0.08794912064420639</v>
       </c>
       <c r="C72">
         <v>0.1064046634549001</v>
@@ -3793,10 +3793,10 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>0.1165189832789967</v>
+        <v>-0.1165189832789967</v>
       </c>
       <c r="B73">
-        <v>0.08829840516434319</v>
+        <v>-0.08829840516434319</v>
       </c>
       <c r="C73">
         <v>0.1129292581072973</v>
@@ -3804,10 +3804,10 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>0.1164835223038357</v>
+        <v>-0.1164835223038357</v>
       </c>
       <c r="B74">
-        <v>0.08873402081478829</v>
+        <v>-0.08873402081478829</v>
       </c>
       <c r="C74">
         <v>0.1181838707213976</v>
@@ -3815,10 +3815,10 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>0.1161133585955221</v>
+        <v>-0.1161133585955221</v>
       </c>
       <c r="B75">
-        <v>0.08928742973560602</v>
+        <v>-0.08928742973560602</v>
       </c>
       <c r="C75">
         <v>0.1222002304440462</v>
@@ -3826,10 +3826,10 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>0.1153600326004128</v>
+        <v>-0.1153600326004128</v>
       </c>
       <c r="B76">
-        <v>0.08997515969433463</v>
+        <v>-0.08997515969433463</v>
       </c>
       <c r="C76">
         <v>0.1249654630556118</v>
@@ -3837,10 +3837,10 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>0.1142107508366547</v>
+        <v>-0.1142107508366547</v>
       </c>
       <c r="B77">
-        <v>0.09077937913561625</v>
+        <v>-0.09077937913561625</v>
       </c>
       <c r="C77">
         <v>0.1264401806783723</v>
@@ -3848,10 +3848,10 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>0.1126825682083056</v>
+        <v>-0.1126825682083056</v>
       </c>
       <c r="B78">
-        <v>0.09165682604283548</v>
+        <v>-0.09165682604283548</v>
       </c>
       <c r="C78">
         <v>0.1266160259530763</v>
@@ -3859,10 +3859,10 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>0.1107830033440867</v>
+        <v>-0.1107830033440867</v>
       </c>
       <c r="B79">
-        <v>0.09257780481077689</v>
+        <v>-0.09257780481077689</v>
       </c>
       <c r="C79">
         <v>0.125503073832637</v>
@@ -3870,10 +3870,10 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>0.1085055254543007</v>
+        <v>-0.1085055254543007</v>
       </c>
       <c r="B80">
-        <v>0.09352514736016554</v>
+        <v>-0.09352514736016554</v>
       </c>
       <c r="C80">
         <v>0.123111794710043</v>
@@ -3881,10 +3881,10 @@
     </row>
     <row r="81">
       <c r="A81">
-        <v>0.1058561845378069</v>
+        <v>-0.1058561845378069</v>
       </c>
       <c r="B81">
-        <v>0.094507625677008</v>
+        <v>-0.094507625677008</v>
       </c>
       <c r="C81">
         <v>0.1194574380080261</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>0.1029004326375739</v>
+        <v>-0.1029004326375739</v>
       </c>
       <c r="B82">
-        <v>0.09554210788087959</v>
+        <v>-0.09554210788087959</v>
       </c>
       <c r="C82">
         <v>0.114543634239492</v>
@@ -3903,10 +3903,10 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>0.09972660611048748</v>
+        <v>-0.09972660611048748</v>
       </c>
       <c r="B83">
-        <v>0.09663984972082268</v>
+        <v>-0.09663984972082268</v>
       </c>
       <c r="C83">
         <v>0.1083706163286962</v>
@@ -3914,10 +3914,10 @@
     </row>
     <row r="84">
       <c r="A84">
-        <v>0.09643932545921344</v>
+        <v>-0.09643932545921344</v>
       </c>
       <c r="B84">
-        <v>0.09782868661638794</v>
+        <v>-0.09782868661638794</v>
       </c>
       <c r="C84">
         <v>0.1009346676710393</v>
@@ -3925,10 +3925,10 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>0.09314302800540604</v>
+        <v>-0.09314302800540604</v>
       </c>
       <c r="B85">
-        <v>0.09911508118732211</v>
+        <v>-0.09911508118732211</v>
       </c>
       <c r="C85">
         <v>0.09222578621432116</v>
@@ -3936,10 +3936,10 @@
     </row>
     <row r="86">
       <c r="A86">
-        <v>0.08992726155678313</v>
+        <v>-0.08992726155678313</v>
       </c>
       <c r="B86">
-        <v>0.1004870424996145</v>
+        <v>-0.1004870424996145</v>
       </c>
       <c r="C86">
         <v>0.08224025680597859</v>
@@ -3947,10 +3947,10 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>0.08682759879198783</v>
+        <v>-0.08682759879198783</v>
       </c>
       <c r="B87">
-        <v>0.1019337996773496</v>
+        <v>-0.1019337996773496</v>
       </c>
       <c r="C87">
         <v>0.07098458371014446</v>
@@ -3958,10 +3958,10 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>0.08385223446502425</v>
+        <v>-0.08385223446502425</v>
       </c>
       <c r="B88">
-        <v>0.1034251543065126</v>
+        <v>-0.1034251543065126</v>
       </c>
       <c r="C88">
         <v>0.05850556509518146</v>
@@ -3969,10 +3969,10 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>0.08099213456433688</v>
+        <v>-0.08099213456433688</v>
       </c>
       <c r="B89">
-        <v>0.1049493052078773</v>
+        <v>-0.1049493052078773</v>
       </c>
       <c r="C89">
         <v>0.04484646919265599</v>
@@ -3980,10 +3980,10 @@
     </row>
     <row r="90">
       <c r="A90">
-        <v>0.07821112937253931</v>
+        <v>-0.07821112937253931</v>
       </c>
       <c r="B90">
-        <v>0.1064995318512713</v>
+        <v>-0.1064995318512713</v>
       </c>
       <c r="C90">
         <v>0.03002327478951087</v>
@@ -3991,10 +3991,10 @@
     </row>
     <row r="91">
       <c r="A91">
-        <v>0.07549164029096311</v>
+        <v>-0.07549164029096311</v>
       </c>
       <c r="B91">
-        <v>0.1080406142607434</v>
+        <v>-0.1080406142607434</v>
       </c>
       <c r="C91">
         <v>0.0140110757383466</v>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="92">
       <c r="A92">
-        <v>0.07282729820659282</v>
+        <v>-0.07282729820659282</v>
       </c>
       <c r="B92">
-        <v>0.1095374372967299</v>
+        <v>-0.1095374372967299</v>
       </c>
       <c r="C92">
         <v>-0.003168391008868944</v>
@@ -4013,10 +4013,10 @@
     </row>
     <row r="93">
       <c r="A93">
-        <v>0.07021113095952444</v>
+        <v>-0.07021113095952444</v>
       </c>
       <c r="B93">
-        <v>0.1109647936065532</v>
+        <v>-0.1109647936065532</v>
       </c>
       <c r="C93">
         <v>-0.02144803826104346</v>
@@ -4024,10 +4024,10 @@
     </row>
     <row r="94">
       <c r="A94">
-        <v>0.06762089429452042</v>
+        <v>-0.06762089429452042</v>
       </c>
       <c r="B94">
-        <v>0.112345955457771</v>
+        <v>-0.112345955457771</v>
       </c>
       <c r="C94">
         <v>-0.04074270098908049</v>
@@ -4035,10 +4035,10 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>0.06503739759682531</v>
+        <v>-0.06503739759682531</v>
       </c>
       <c r="B95">
-        <v>0.1137260557441816</v>
+        <v>-0.1137260557441816</v>
       </c>
       <c r="C95">
         <v>-0.06090185040425431</v>
@@ -4046,10 +4046,10 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>0.06243172487795604</v>
+        <v>-0.06243172487795604</v>
       </c>
       <c r="B96">
-        <v>0.1151703019371564</v>
+        <v>-0.1151703019371564</v>
       </c>
       <c r="C96">
         <v>-0.08174312895249447</v>
@@ -4057,10 +4057,10 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>0.0597821937546212</v>
+        <v>-0.0597821937546212</v>
       </c>
       <c r="B97">
-        <v>0.1167258112654936</v>
+        <v>-0.1167258112654936</v>
       </c>
       <c r="C97">
         <v>-0.1030926656380046</v>
@@ -4068,10 +4068,10 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>0.05709641232384591</v>
+        <v>-0.05709641232384591</v>
       </c>
       <c r="B98">
-        <v>0.1184114728822742</v>
+        <v>-0.1184114728822742</v>
       </c>
       <c r="C98">
         <v>-0.1247984366025859</v>
@@ -4079,10 +4079,10 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>0.05439349716927407</v>
+        <v>-0.05439349716927407</v>
       </c>
       <c r="B99">
-        <v>0.120247064547529</v>
+        <v>-0.120247064547529</v>
       </c>
       <c r="C99">
         <v>-0.1467528425026699</v>
@@ -4090,10 +4090,10 @@
     </row>
     <row r="100">
       <c r="A100">
-        <v>0.05169250713897352</v>
+        <v>-0.05169250713897352</v>
       </c>
       <c r="B100">
-        <v>0.1221997950482935</v>
+        <v>-0.1221997950482935</v>
       </c>
       <c r="C100">
         <v>-0.1688494854745694</v>
@@ -4101,10 +4101,10 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>0.04899273549016162</v>
+        <v>-0.04899273549016162</v>
       </c>
       <c r="B101">
-        <v>0.1242072483619488</v>
+        <v>-0.1242072483619488</v>
       </c>
       <c r="C101">
         <v>-0.1909998643960533</v>
@@ -4112,10 +4112,10 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>0.04628588245930788</v>
+        <v>-0.04628588245930788</v>
       </c>
       <c r="B102">
-        <v>0.1262396896588266</v>
+        <v>-0.1262396896588266</v>
       </c>
       <c r="C102">
         <v>-0.2131636456649294</v>

</xml_diff>

<commit_message>
change output variable names
</commit_message>
<xml_diff>
--- a/figure_table/toyexample_TEMPTED.xlsx
+++ b/figure_table/toyexample_TEMPTED.xlsx
@@ -7,13 +7,13 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="A.hat" sheetId="1" r:id="rId1"/>
-    <sheet name="B.hat" sheetId="2" r:id="rId2"/>
-    <sheet name="Phi.hat" sheetId="3" r:id="rId3"/>
-    <sheet name="time" sheetId="4" r:id="rId4"/>
+    <sheet name="A_hat" sheetId="1" r:id="rId1"/>
+    <sheet name="B_hat" sheetId="2" r:id="rId2"/>
+    <sheet name="Phi_hat" sheetId="3" r:id="rId3"/>
+    <sheet name="time_Phi" sheetId="4" r:id="rId4"/>
     <sheet name="Lambda" sheetId="5" r:id="rId5"/>
-    <sheet name="r.square" sheetId="6" r:id="rId6"/>
-    <sheet name="accum.r.square" sheetId="7" r:id="rId7"/>
+    <sheet name="r_square" sheetId="6" r:id="rId6"/>
+    <sheet name="accum_r_square" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -392,10 +392,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.07880033100398944</v>
+        <v>-0.07880033100398944</v>
       </c>
       <c r="C2">
-        <v>-0.1214369994391653</v>
+        <v>0.1214369994391653</v>
       </c>
       <c r="D2">
         <v>0.08286637801416286</v>
@@ -408,10 +408,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.1597047368379094</v>
+        <v>-0.1597047368379094</v>
       </c>
       <c r="C3">
-        <v>-0.08924064136581804</v>
+        <v>0.08924064136581804</v>
       </c>
       <c r="D3">
         <v>0.02194583339231184</v>
@@ -424,10 +424,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.09182320861932254</v>
+        <v>-0.09182320861932254</v>
       </c>
       <c r="C4">
-        <v>-0.1399065702590379</v>
+        <v>0.1399065702590379</v>
       </c>
       <c r="D4">
         <v>0.08142219514737449</v>
@@ -440,10 +440,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.06885075539748635</v>
+        <v>-0.06885075539748635</v>
       </c>
       <c r="C5">
-        <v>-0.1507682320556845</v>
+        <v>0.1507682320556845</v>
       </c>
       <c r="D5">
         <v>0.1828830105495226</v>
@@ -456,10 +456,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.1064637437162154</v>
+        <v>-0.1064637437162154</v>
       </c>
       <c r="C6">
-        <v>-0.2004787865145692</v>
+        <v>0.2004787865145692</v>
       </c>
       <c r="D6">
         <v>0.1593372006206886</v>
@@ -472,10 +472,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.08468212103776607</v>
+        <v>-0.08468212103776607</v>
       </c>
       <c r="C7">
-        <v>-0.231414938101536</v>
+        <v>0.231414938101536</v>
       </c>
       <c r="D7">
         <v>0.1374942494335623</v>
@@ -488,10 +488,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.006942093937174086</v>
+        <v>-0.006942093937174086</v>
       </c>
       <c r="C8">
-        <v>-0.1569134902252004</v>
+        <v>0.1569134902252004</v>
       </c>
       <c r="D8">
         <v>0.1709881830670296</v>
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.1181267850122958</v>
+        <v>-0.1181267850122958</v>
       </c>
       <c r="C9">
-        <v>-0.1579221650765876</v>
+        <v>0.1579221650765876</v>
       </c>
       <c r="D9">
         <v>0.08154890345050997</v>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.03989675258009495</v>
+        <v>-0.03989675258009495</v>
       </c>
       <c r="C10">
-        <v>-0.149923486753858</v>
+        <v>0.149923486753858</v>
       </c>
       <c r="D10">
         <v>0.181058889512264</v>
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.03398321206824673</v>
+        <v>-0.03398321206824673</v>
       </c>
       <c r="C11">
-        <v>-0.1325572000438724</v>
+        <v>0.1325572000438724</v>
       </c>
       <c r="D11">
         <v>0.09324971122061536</v>
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.0393834362513036</v>
+        <v>-0.0393834362513036</v>
       </c>
       <c r="C12">
-        <v>-0.1069070723376464</v>
+        <v>0.1069070723376464</v>
       </c>
       <c r="D12">
         <v>0.06029063684868469</v>
@@ -568,10 +568,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.06418415895501667</v>
+        <v>-0.06418415895501667</v>
       </c>
       <c r="C13">
-        <v>-0.1279859881148709</v>
+        <v>0.1279859881148709</v>
       </c>
       <c r="D13">
         <v>0.1195667273895422</v>
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.07242971303684753</v>
+        <v>-0.07242971303684753</v>
       </c>
       <c r="C14">
-        <v>-0.1494128835333963</v>
+        <v>0.1494128835333963</v>
       </c>
       <c r="D14">
         <v>0.04266706133200412</v>
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.09029877826118225</v>
+        <v>-0.09029877826118225</v>
       </c>
       <c r="C15">
-        <v>-0.1625674025572098</v>
+        <v>0.1625674025572098</v>
       </c>
       <c r="D15">
         <v>0.05610808754397775</v>
@@ -616,10 +616,10 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.0326595669318467</v>
+        <v>-0.0326595669318467</v>
       </c>
       <c r="C16">
-        <v>-0.1491304409524304</v>
+        <v>0.1491304409524304</v>
       </c>
       <c r="D16">
         <v>0.08068434163336682</v>
@@ -632,10 +632,10 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.05572218326875031</v>
+        <v>-0.05572218326875031</v>
       </c>
       <c r="C17">
-        <v>-0.1282802804216011</v>
+        <v>0.1282802804216011</v>
       </c>
       <c r="D17">
         <v>0.06982946815661424</v>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.1188887401453342</v>
+        <v>-0.1188887401453342</v>
       </c>
       <c r="C18">
-        <v>-0.196080812070059</v>
+        <v>0.196080812070059</v>
       </c>
       <c r="D18">
         <v>0.08348757761444664</v>
@@ -664,10 +664,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.09593907800657581</v>
+        <v>-0.09593907800657581</v>
       </c>
       <c r="C19">
-        <v>-0.1112069989509569</v>
+        <v>0.1112069989509569</v>
       </c>
       <c r="D19">
         <v>0.2161882178419718</v>
@@ -680,10 +680,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.059080270576451</v>
+        <v>-0.059080270576451</v>
       </c>
       <c r="C20">
-        <v>-0.1287622198577844</v>
+        <v>0.1287622198577844</v>
       </c>
       <c r="D20">
         <v>0.06929104037800883</v>
@@ -696,10 +696,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.1086246116494793</v>
+        <v>-0.1086246116494793</v>
       </c>
       <c r="C21">
-        <v>-0.2478063645090004</v>
+        <v>0.2478063645090004</v>
       </c>
       <c r="D21">
         <v>0.1040687696044373</v>
@@ -712,10 +712,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.1207840450460627</v>
+        <v>-0.1207840450460627</v>
       </c>
       <c r="C22">
-        <v>-0.0400602660338118</v>
+        <v>0.0400602660338118</v>
       </c>
       <c r="D22">
         <v>0.1523271192084657</v>
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.1424967482471836</v>
+        <v>-0.1424967482471836</v>
       </c>
       <c r="C23">
-        <v>0.04804290026338388</v>
+        <v>-0.04804290026338388</v>
       </c>
       <c r="D23">
         <v>0.1215239350647906</v>
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.1841318024115703</v>
+        <v>-0.1841318024115703</v>
       </c>
       <c r="C24">
-        <v>-0.05304303404014515</v>
+        <v>0.05304303404014515</v>
       </c>
       <c r="D24">
         <v>0.1052458977956333</v>
@@ -760,10 +760,10 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.1880883407097291</v>
+        <v>-0.1880883407097291</v>
       </c>
       <c r="C25">
-        <v>-0.04652472903038417</v>
+        <v>0.04652472903038417</v>
       </c>
       <c r="D25">
         <v>0.07786685759590449</v>
@@ -776,10 +776,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.1166535035664137</v>
+        <v>-0.1166535035664137</v>
       </c>
       <c r="C26">
-        <v>-0.05331014115494709</v>
+        <v>0.05331014115494709</v>
       </c>
       <c r="D26">
         <v>0.1084221622006323</v>
@@ -792,10 +792,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.1489222249139132</v>
+        <v>-0.1489222249139132</v>
       </c>
       <c r="C27">
-        <v>-0.01787104103422705</v>
+        <v>0.01787104103422705</v>
       </c>
       <c r="D27">
         <v>0.1304433213087429</v>
@@ -808,10 +808,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.1361027041258603</v>
+        <v>-0.1361027041258603</v>
       </c>
       <c r="C28">
-        <v>0.04405263595672025</v>
+        <v>-0.04405263595672025</v>
       </c>
       <c r="D28">
         <v>0.1052854343647315</v>
@@ -824,10 +824,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.1246603111788643</v>
+        <v>-0.1246603111788643</v>
       </c>
       <c r="C29">
-        <v>0.004160658796581899</v>
+        <v>-0.004160658796581899</v>
       </c>
       <c r="D29">
         <v>0.09807544077649784</v>
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>0.1574420473153161</v>
+        <v>-0.1574420473153161</v>
       </c>
       <c r="C30">
-        <v>-0.06313717410600292</v>
+        <v>0.06313717410600292</v>
       </c>
       <c r="D30">
         <v>0.1041393907348075</v>
@@ -856,10 +856,10 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.1060189038618903</v>
+        <v>-0.1060189038618903</v>
       </c>
       <c r="C31">
-        <v>-0.08657780365855253</v>
+        <v>0.08657780365855253</v>
       </c>
       <c r="D31">
         <v>0.04694756544500957</v>
@@ -872,10 +872,10 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.1568412589673558</v>
+        <v>-0.1568412589673558</v>
       </c>
       <c r="C32">
-        <v>0.0087038431122955</v>
+        <v>-0.0087038431122955</v>
       </c>
       <c r="D32">
         <v>0.09739018354220523</v>
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.1518207445508232</v>
+        <v>-0.1518207445508232</v>
       </c>
       <c r="C33">
-        <v>-0.01938041579834017</v>
+        <v>0.01938041579834017</v>
       </c>
       <c r="D33">
         <v>0.1035820134209568</v>
@@ -904,10 +904,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.08476183168910413</v>
+        <v>-0.08476183168910413</v>
       </c>
       <c r="C34">
-        <v>0.0488533308951106</v>
+        <v>-0.0488533308951106</v>
       </c>
       <c r="D34">
         <v>0.09051974234979543</v>
@@ -920,10 +920,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.1904791751848131</v>
+        <v>-0.1904791751848131</v>
       </c>
       <c r="C35">
-        <v>0.006666381894677296</v>
+        <v>-0.006666381894677296</v>
       </c>
       <c r="D35">
         <v>0.1115794817294884</v>
@@ -936,10 +936,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.1197296066625953</v>
+        <v>-0.1197296066625953</v>
       </c>
       <c r="C36">
-        <v>0.04137040799836017</v>
+        <v>-0.04137040799836017</v>
       </c>
       <c r="D36">
         <v>0.191588624992434</v>
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.09845232729245383</v>
+        <v>-0.09845232729245383</v>
       </c>
       <c r="C37">
-        <v>-0.02353201588609518</v>
+        <v>0.02353201588609518</v>
       </c>
       <c r="D37">
         <v>0.2011007193876927</v>
@@ -968,10 +968,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.1504012091219676</v>
+        <v>-0.1504012091219676</v>
       </c>
       <c r="C38">
-        <v>0.02765697563870612</v>
+        <v>-0.02765697563870612</v>
       </c>
       <c r="D38">
         <v>0.100213658553973</v>
@@ -984,10 +984,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.07122830914109726</v>
+        <v>-0.07122830914109726</v>
       </c>
       <c r="C39">
-        <v>-0.07506640441448975</v>
+        <v>0.07506640441448975</v>
       </c>
       <c r="D39">
         <v>0.2206316210571686</v>
@@ -1000,10 +1000,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.2265197967315946</v>
+        <v>-0.2265197967315946</v>
       </c>
       <c r="C40">
-        <v>0.04740057954479043</v>
+        <v>-0.04740057954479043</v>
       </c>
       <c r="D40">
         <v>0.01361621534738438</v>
@@ -1016,10 +1016,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.1613174140009147</v>
+        <v>-0.1613174140009147</v>
       </c>
       <c r="C41">
-        <v>0.009525502976460364</v>
+        <v>-0.009525502976460364</v>
       </c>
       <c r="D41">
         <v>0.1016482954363994</v>
@@ -1032,10 +1032,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>-0.1524815940947832</v>
+        <v>0.1524815940947832</v>
       </c>
       <c r="C42">
-        <v>-0.09539351800340515</v>
+        <v>0.09539351800340515</v>
       </c>
       <c r="D42">
         <v>0.07907566791150117</v>
@@ -1048,10 +1048,10 @@
         </is>
       </c>
       <c r="B43">
-        <v>-0.1006952260212896</v>
+        <v>0.1006952260212896</v>
       </c>
       <c r="C43">
-        <v>-0.1754087969904064</v>
+        <v>0.1754087969904064</v>
       </c>
       <c r="D43">
         <v>0.1010814514830914</v>
@@ -1064,10 +1064,10 @@
         </is>
       </c>
       <c r="B44">
-        <v>-0.1297706116613269</v>
+        <v>0.1297706116613269</v>
       </c>
       <c r="C44">
-        <v>-0.16258805335235</v>
+        <v>0.16258805335235</v>
       </c>
       <c r="D44">
         <v>0.1126153295510959</v>
@@ -1080,10 +1080,10 @@
         </is>
       </c>
       <c r="B45">
-        <v>-0.06887893405855348</v>
+        <v>0.06887893405855348</v>
       </c>
       <c r="C45">
-        <v>-0.2011623620254935</v>
+        <v>0.2011623620254935</v>
       </c>
       <c r="D45">
         <v>0.1052471457489279</v>
@@ -1096,10 +1096,10 @@
         </is>
       </c>
       <c r="B46">
-        <v>-0.1286975011557017</v>
+        <v>0.1286975011557017</v>
       </c>
       <c r="C46">
-        <v>-0.1366386636569925</v>
+        <v>0.1366386636569925</v>
       </c>
       <c r="D46">
         <v>0.1089611643971406</v>
@@ -1112,10 +1112,10 @@
         </is>
       </c>
       <c r="B47">
-        <v>-0.1391387690211929</v>
+        <v>0.1391387690211929</v>
       </c>
       <c r="C47">
-        <v>-0.1430096268577066</v>
+        <v>0.1430096268577066</v>
       </c>
       <c r="D47">
         <v>0.1007542559006574</v>
@@ -1128,10 +1128,10 @@
         </is>
       </c>
       <c r="B48">
-        <v>-0.08871823613264167</v>
+        <v>0.08871823613264167</v>
       </c>
       <c r="C48">
-        <v>-0.2535098651157587</v>
+        <v>0.2535098651157587</v>
       </c>
       <c r="D48">
         <v>0.1150785997162549</v>
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="B49">
-        <v>-0.1877606920033705</v>
+        <v>0.1877606920033705</v>
       </c>
       <c r="C49">
-        <v>-0.1148520871673355</v>
+        <v>0.1148520871673355</v>
       </c>
       <c r="D49">
         <v>0.201843583806864</v>
@@ -1160,10 +1160,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>-0.1569417085128846</v>
+        <v>0.1569417085128846</v>
       </c>
       <c r="C50">
-        <v>-0.1367260694464659</v>
+        <v>0.1367260694464659</v>
       </c>
       <c r="D50">
         <v>0.2812543447786442</v>
@@ -1176,10 +1176,10 @@
         </is>
       </c>
       <c r="B51">
-        <v>-0.1594157473842039</v>
+        <v>0.1594157473842039</v>
       </c>
       <c r="C51">
-        <v>-0.126431634358593</v>
+        <v>0.126431634358593</v>
       </c>
       <c r="D51">
         <v>0.222429672884922</v>
@@ -1192,10 +1192,10 @@
         </is>
       </c>
       <c r="B52">
-        <v>-0.166420343368233</v>
+        <v>0.166420343368233</v>
       </c>
       <c r="C52">
-        <v>-0.1029979520168319</v>
+        <v>0.1029979520168319</v>
       </c>
       <c r="D52">
         <v>0.1730408711989471</v>
@@ -1208,10 +1208,10 @@
         </is>
       </c>
       <c r="B53">
-        <v>-0.1389604624739776</v>
+        <v>0.1389604624739776</v>
       </c>
       <c r="C53">
-        <v>-0.07987778110635416</v>
+        <v>0.07987778110635416</v>
       </c>
       <c r="D53">
         <v>0.07531211867155593</v>
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B54">
-        <v>-0.09480884968176284</v>
+        <v>0.09480884968176284</v>
       </c>
       <c r="C54">
-        <v>-0.136970448380681</v>
+        <v>0.136970448380681</v>
       </c>
       <c r="D54">
         <v>0.1058745716315293</v>
@@ -1240,10 +1240,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>-0.171837564703721</v>
+        <v>0.171837564703721</v>
       </c>
       <c r="C55">
-        <v>-0.1385598712777725</v>
+        <v>0.1385598712777725</v>
       </c>
       <c r="D55">
         <v>0.1060105896373873</v>
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>-0.192171193283747</v>
+        <v>0.192171193283747</v>
       </c>
       <c r="C56">
-        <v>-0.1387569041945457</v>
+        <v>0.1387569041945457</v>
       </c>
       <c r="D56">
         <v>0.1729712366942464</v>
@@ -1272,10 +1272,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>-0.2048876041419146</v>
+        <v>0.2048876041419146</v>
       </c>
       <c r="C57">
-        <v>-0.08165555404799489</v>
+        <v>0.08165555404799489</v>
       </c>
       <c r="D57">
         <v>0.1692860454501073</v>
@@ -1288,10 +1288,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>-0.1636535110991047</v>
+        <v>0.1636535110991047</v>
       </c>
       <c r="C58">
-        <v>-0.1410792001829381</v>
+        <v>0.1410792001829381</v>
       </c>
       <c r="D58">
         <v>0.1310094319869677</v>
@@ -1304,10 +1304,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>-0.09529976887725825</v>
+        <v>0.09529976887725825</v>
       </c>
       <c r="C59">
-        <v>-0.1489229712502358</v>
+        <v>0.1489229712502358</v>
       </c>
       <c r="D59">
         <v>0.08593932294132844</v>
@@ -1320,10 +1320,10 @@
         </is>
       </c>
       <c r="B60">
-        <v>-0.1704178216584816</v>
+        <v>0.1704178216584816</v>
       </c>
       <c r="C60">
-        <v>-0.1004813114613144</v>
+        <v>0.1004813114613144</v>
       </c>
       <c r="D60">
         <v>0.09599681296790769</v>
@@ -1336,10 +1336,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>-0.1198211957719144</v>
+        <v>0.1198211957719144</v>
       </c>
       <c r="C61">
-        <v>-0.277698010227947</v>
+        <v>0.277698010227947</v>
       </c>
       <c r="D61">
         <v>0.1649019368160083</v>
@@ -3012,10 +3012,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-0.03584611425551176</v>
+        <v>0.03584611425551176</v>
       </c>
       <c r="B2">
-        <v>0.1261660229675725</v>
+        <v>-0.1261660229675725</v>
       </c>
       <c r="C2">
         <v>-0.2114090648450627</v>
@@ -3023,10 +3023,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>-0.03888348454188601</v>
+        <v>0.03888348454188601</v>
       </c>
       <c r="B3">
-        <v>0.1280966100874439</v>
+        <v>-0.1280966100874439</v>
       </c>
       <c r="C3">
         <v>-0.1908208461452241</v>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>-0.04190078771077085</v>
+        <v>0.04190078771077085</v>
       </c>
       <c r="B4">
-        <v>0.1300479773889831</v>
+        <v>-0.1300479773889831</v>
       </c>
       <c r="C4">
         <v>-0.1702523380531559</v>
@@ -3045,10 +3045,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>-0.04485766930607214</v>
+        <v>0.04485766930607214</v>
       </c>
       <c r="B5">
-        <v>0.1320303666728868</v>
+        <v>-0.1320303666728868</v>
       </c>
       <c r="C5">
         <v>-0.1497399351875364</v>
@@ -3056,10 +3056,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>-0.04771968755473609</v>
+        <v>0.04771968755473609</v>
       </c>
       <c r="B6">
-        <v>0.1340030946923663</v>
+        <v>-0.1340030946923663</v>
       </c>
       <c r="C6">
         <v>-0.1293541106290052</v>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>-0.05049449189690745</v>
+        <v>0.05049449189690745</v>
       </c>
       <c r="B7">
-        <v>0.1358767400937768</v>
+        <v>-0.1358767400937768</v>
       </c>
       <c r="C7">
         <v>-0.1091667532894945</v>
@@ -3078,10 +3078,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>-0.05323720007498162</v>
+        <v>0.05323720007498162</v>
       </c>
       <c r="B8">
-        <v>0.1375873429855182</v>
+        <v>-0.1375873429855182</v>
       </c>
       <c r="C8">
         <v>-0.08923731780255828</v>
@@ -3089,10 +3089,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>-0.05602764123582211</v>
+        <v>0.05602764123582211</v>
       </c>
       <c r="B9">
-        <v>0.139112344381051</v>
+        <v>-0.139112344381051</v>
       </c>
       <c r="C9">
         <v>-0.06960621210965814</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>-0.05891856211600118</v>
+        <v>0.05891856211600118</v>
       </c>
       <c r="B10">
-        <v>0.1403709563575088</v>
+        <v>-0.1403709563575088</v>
       </c>
       <c r="C10">
         <v>-0.05037354421408783</v>
@@ -3111,10 +3111,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>-0.06192080305161932</v>
+        <v>0.06192080305161932</v>
       </c>
       <c r="B11">
-        <v>0.1412620094606763</v>
+        <v>-0.1412620094606763</v>
       </c>
       <c r="C11">
         <v>-0.03166623998205532</v>
@@ -3122,10 +3122,10 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>-0.06502997221068191</v>
+        <v>0.06502997221068191</v>
       </c>
       <c r="B12">
-        <v>0.1417049914353085</v>
+        <v>-0.1417049914353085</v>
       </c>
       <c r="C12">
         <v>-0.0136124037126967</v>
@@ -3133,10 +3133,10 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>-0.0682217927374613</v>
+        <v>0.0682217927374613</v>
       </c>
       <c r="B13">
-        <v>0.1417017789286655</v>
+        <v>-0.1417017789286655</v>
       </c>
       <c r="C13">
         <v>0.003655262130591408</v>
@@ -3144,10 +3144,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>-0.07147981864187419</v>
+        <v>0.07147981864187419</v>
       </c>
       <c r="B14">
-        <v>0.1412829067322424</v>
+        <v>-0.1412829067322424</v>
       </c>
       <c r="C14">
         <v>0.02002067260579577</v>
@@ -3155,10 +3155,10 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>-0.07479378898660065</v>
+        <v>0.07479378898660065</v>
       </c>
       <c r="B15">
-        <v>0.1404766937034764</v>
+        <v>-0.1404766937034764</v>
       </c>
       <c r="C15">
         <v>0.03541008150476255</v>
@@ -3166,10 +3166,10 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>-0.07813776785780477</v>
+        <v>0.07813776785780477</v>
       </c>
       <c r="B16">
-        <v>0.1393327134303599</v>
+        <v>-0.1393327134303599</v>
       </c>
       <c r="C16">
         <v>0.04973524646842393</v>
@@ -3177,10 +3177,10 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>-0.0814609933235251</v>
+        <v>0.0814609933235251</v>
       </c>
       <c r="B17">
-        <v>0.1379115473026885</v>
+        <v>-0.1379115473026885</v>
       </c>
       <c r="C17">
         <v>0.06291090653511749</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>-0.0847460889320646</v>
+        <v>0.0847460889320646</v>
       </c>
       <c r="B18">
-        <v>0.1362359448069206</v>
+        <v>-0.1362359448069206</v>
       </c>
       <c r="C18">
         <v>0.07489361441684624</v>
@@ -3199,10 +3199,10 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>-0.08798957340369122</v>
+        <v>0.08798957340369122</v>
       </c>
       <c r="B19">
-        <v>0.13431261277634</v>
+        <v>-0.13431261277634</v>
       </c>
       <c r="C19">
         <v>0.08567338841457367</v>
@@ -3210,10 +3210,10 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>-0.09116892161060079</v>
+        <v>0.09116892161060079</v>
       </c>
       <c r="B20">
-        <v>0.1321639880710429</v>
+        <v>-0.1321639880710429</v>
       </c>
       <c r="C20">
         <v>0.0952191600999244</v>
@@ -3221,10 +3221,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>-0.09425152007691803</v>
+        <v>0.09425152007691803</v>
       </c>
       <c r="B21">
-        <v>0.129792202374663</v>
+        <v>-0.129792202374663</v>
       </c>
       <c r="C21">
         <v>0.1034293501194486</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>-0.09718356612790389</v>
+        <v>0.09718356612790389</v>
       </c>
       <c r="B22">
-        <v>0.1271917421652431</v>
+        <v>-0.1271917421652431</v>
       </c>
       <c r="C22">
         <v>0.1101934723703826</v>
@@ -3243,10 +3243,10 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>-0.0999147371795141</v>
+        <v>0.0999147371795141</v>
       </c>
       <c r="B23">
-        <v>0.1243474336847771</v>
+        <v>-0.1243474336847771</v>
       </c>
       <c r="C23">
         <v>0.1154325310850253</v>
@@ -3254,10 +3254,10 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>-0.1024411458943892</v>
+        <v>0.1024411458943892</v>
       </c>
       <c r="B24">
-        <v>0.1212491236992373</v>
+        <v>-0.1212491236992373</v>
       </c>
       <c r="C24">
         <v>0.1191109387747327</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>-0.104758855565474</v>
+        <v>0.104758855565474</v>
       </c>
       <c r="B25">
-        <v>0.1178570458575076</v>
+        <v>-0.1178570458575076</v>
       </c>
       <c r="C25">
         <v>0.121241093243928</v>
@@ -3276,10 +3276,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>-0.1068821113627917</v>
+        <v>0.1068821113627917</v>
       </c>
       <c r="B26">
-        <v>0.1141234166013049</v>
+        <v>-0.1141234166013049</v>
       </c>
       <c r="C26">
         <v>0.1218533141761865</v>
@@ -3287,10 +3287,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>-0.1088122123022573</v>
+        <v>0.1088122123022573</v>
       </c>
       <c r="B27">
-        <v>0.1100091261522422</v>
+        <v>-0.1100091261522422</v>
       </c>
       <c r="C27">
         <v>0.1210042011080165</v>
@@ -3298,10 +3298,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>-0.1104941612425646</v>
+        <v>0.1104941612425646</v>
       </c>
       <c r="B28">
-        <v>0.1054996126930566</v>
+        <v>-0.1054996126930566</v>
       </c>
       <c r="C28">
         <v>0.1187307541634631</v>
@@ -3309,10 +3309,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>-0.1118783610632255</v>
+        <v>0.1118783610632255</v>
       </c>
       <c r="B29">
-        <v>0.1006290414523116</v>
+        <v>-0.1006290414523116</v>
       </c>
       <c r="C29">
         <v>0.1150658859673596</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>-0.1129648114253242</v>
+        <v>0.1129648114253242</v>
       </c>
       <c r="B30">
-        <v>0.09542311040749513</v>
+        <v>-0.09542311040749513</v>
       </c>
       <c r="C30">
         <v>0.1100693033274244</v>
@@ -3331,10 +3331,10 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>-0.1137631319739484</v>
+        <v>0.1137631319739484</v>
       </c>
       <c r="B31">
-        <v>0.0898902283505609</v>
+        <v>-0.0898902283505609</v>
       </c>
       <c r="C31">
         <v>0.1038190413265975</v>
@@ -3342,10 +3342,10 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>-0.1142600113166586</v>
+        <v>0.1142600113166586</v>
       </c>
       <c r="B32">
-        <v>0.08402796676416481</v>
+        <v>-0.08402796676416481</v>
       </c>
       <c r="C32">
         <v>0.09636623408259679</v>
@@ -3353,10 +3353,10 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>-0.1144563690838302</v>
+        <v>0.1144563690838302</v>
       </c>
       <c r="B33">
-        <v>0.07785485117788461</v>
+        <v>-0.07785485117788461</v>
       </c>
       <c r="C33">
         <v>0.08777310153522087</v>
@@ -3364,10 +3364,10 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>-0.1144043171831065</v>
+        <v>0.1144043171831065</v>
       </c>
       <c r="B34">
-        <v>0.07138520866556547</v>
+        <v>-0.07138520866556547</v>
       </c>
       <c r="C34">
         <v>0.07810488671683126</v>
@@ -3375,10 +3375,10 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>-0.1142021332788516</v>
+        <v>0.1142021332788516</v>
       </c>
       <c r="B35">
-        <v>0.06460178118966367</v>
+        <v>-0.06460178118966367</v>
       </c>
       <c r="C35">
         <v>0.067394993701182</v>
@@ -3386,10 +3386,10 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>-0.1139490195579526</v>
+        <v>0.1139490195579526</v>
       </c>
       <c r="B36">
-        <v>0.05753619880781555</v>
+        <v>-0.05753619880781555</v>
       </c>
       <c r="C36">
         <v>0.05569652325763148</v>
@@ -3397,10 +3397,10 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>-0.1137118752692501</v>
+        <v>0.1137118752692501</v>
       </c>
       <c r="B37">
-        <v>0.05024153762267213</v>
+        <v>-0.05024153762267213</v>
       </c>
       <c r="C37">
         <v>0.04310554140968866</v>
@@ -3408,10 +3408,10 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>-0.1135261950400183</v>
+        <v>0.1135261950400183</v>
       </c>
       <c r="B38">
-        <v>0.0427547203437779</v>
+        <v>-0.0427547203437779</v>
       </c>
       <c r="C38">
         <v>0.02972379916907733</v>
@@ -3419,10 +3419,10 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>-0.1133952595789638</v>
+        <v>0.1133952595789638</v>
       </c>
       <c r="B39">
-        <v>0.03510418176991831</v>
+        <v>-0.03510418176991831</v>
       </c>
       <c r="C39">
         <v>0.01564281432055305</v>
@@ -3430,10 +3430,10 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>-0.1133439230422368</v>
+        <v>0.1133439230422368</v>
       </c>
       <c r="B40">
-        <v>0.02734071614690875</v>
+        <v>-0.02734071614690875</v>
       </c>
       <c r="C40">
         <v>0.0009725763272283479</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>-0.1134246352605632</v>
+        <v>0.1134246352605632</v>
       </c>
       <c r="B41">
-        <v>0.01951218510840367</v>
+        <v>-0.01951218510840367</v>
       </c>
       <c r="C41">
         <v>-0.01414504278215793</v>
@@ -3452,10 +3452,10 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>-0.1136633701498238</v>
+        <v>0.1136633701498238</v>
       </c>
       <c r="B42">
-        <v>0.01164778875484332</v>
+        <v>-0.01164778875484332</v>
       </c>
       <c r="C42">
         <v>-0.02952782495901124</v>
@@ -3463,10 +3463,10 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>-0.1140692530327002</v>
+        <v>0.1140692530327002</v>
       </c>
       <c r="B43">
-        <v>0.003777014572843958</v>
+        <v>-0.003777014572843958</v>
       </c>
       <c r="C43">
         <v>-0.04494157995906006</v>
@@ -3474,10 +3474,10 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>-0.114672925563359</v>
+        <v>0.114672925563359</v>
       </c>
       <c r="B44">
-        <v>-0.004068177303939098</v>
+        <v>0.004068177303939098</v>
       </c>
       <c r="C44">
         <v>-0.06013259652916059</v>
@@ -3485,10 +3485,10 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>-0.1154931671130773</v>
+        <v>0.1154931671130773</v>
       </c>
       <c r="B45">
-        <v>-0.01183029205118377</v>
+        <v>0.01183029205118377</v>
       </c>
       <c r="C45">
         <v>-0.07484772120854274</v>
@@ -3496,10 +3496,10 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>-0.1165305508495583</v>
+        <v>0.1165305508495583</v>
       </c>
       <c r="B46">
-        <v>-0.01943297374775248</v>
+        <v>0.01943297374775248</v>
       </c>
       <c r="C46">
         <v>-0.08881738572507106</v>
@@ -3507,10 +3507,10 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>-0.1177269485186222</v>
+        <v>0.1177269485186222</v>
       </c>
       <c r="B47">
-        <v>-0.02677774852663677</v>
+        <v>0.02677774852663677</v>
       </c>
       <c r="C47">
         <v>-0.1016883764341552</v>
@@ -3518,10 +3518,10 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>-0.119006967533228</v>
+        <v>0.119006967533228</v>
       </c>
       <c r="B48">
-        <v>-0.03375224609691165</v>
+        <v>0.03375224609691165</v>
       </c>
       <c r="C48">
         <v>-0.1130355815372494</v>
@@ -3529,10 +3529,10 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>-0.1202839163487873</v>
+        <v>0.1202839163487873</v>
       </c>
       <c r="B49">
-        <v>-0.04028312045368849</v>
+        <v>0.04028312045368849</v>
       </c>
       <c r="C49">
         <v>-0.1223924603423906</v>
@@ -3540,10 +3540,10 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>-0.1214556379485759</v>
+        <v>0.1214556379485759</v>
       </c>
       <c r="B50">
-        <v>-0.04631668941238382</v>
+        <v>0.04631668941238382</v>
       </c>
       <c r="C50">
         <v>-0.129313710328427</v>
@@ -3551,10 +3551,10 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>-0.1224057849476866</v>
+        <v>0.1224057849476866</v>
       </c>
       <c r="B51">
-        <v>-0.05182533663358131</v>
+        <v>0.05182533663358131</v>
       </c>
       <c r="C51">
         <v>-0.1334666994811328</v>
@@ -3562,10 +3562,10 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>-0.1230491140443012</v>
+        <v>0.1230491140443012</v>
       </c>
       <c r="B52">
-        <v>-0.05681894029754148</v>
+        <v>0.05681894029754148</v>
       </c>
       <c r="C52">
         <v>-0.1347448387520708</v>
@@ -3573,10 +3573,10 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>-0.1233268227003705</v>
+        <v>0.1233268227003705</v>
       </c>
       <c r="B53">
-        <v>-0.06128894727673403</v>
+        <v>0.06128894727673403</v>
       </c>
       <c r="C53">
         <v>-0.1331586796052998</v>
@@ -3584,10 +3584,10 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>-0.1232366792821226</v>
+        <v>0.1232366792821226</v>
       </c>
       <c r="B54">
-        <v>-0.06523553971000566</v>
+        <v>0.06523553971000566</v>
       </c>
       <c r="C54">
         <v>-0.1287576585669029</v>
@@ -3595,10 +3595,10 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>-0.1228353195153089</v>
+        <v>0.1228353195153089</v>
       </c>
       <c r="B55">
-        <v>-0.06871843866654584</v>
+        <v>0.06871843866654584</v>
       </c>
       <c r="C55">
         <v>-0.1217150605764785</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>-0.1221954001912476</v>
+        <v>0.1221954001912476</v>
       </c>
       <c r="B56">
-        <v>-0.07184939491094641</v>
+        <v>0.07184939491094641</v>
       </c>
       <c r="C56">
         <v>-0.1123102085723662</v>
@@ -3617,10 +3617,10 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>-0.1214031333606612</v>
+        <v>0.1214031333606612</v>
       </c>
       <c r="B57">
-        <v>-0.07470037737350561</v>
+        <v>0.07470037737350561</v>
       </c>
       <c r="C57">
         <v>-0.1008490075047416</v>
@@ -3628,10 +3628,10 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>-0.1205248045267173</v>
+        <v>0.1205248045267173</v>
       </c>
       <c r="B58">
-        <v>-0.07730515374469728</v>
+        <v>0.07730515374469728</v>
       </c>
       <c r="C58">
         <v>-0.08764487787861819</v>
@@ -3639,10 +3639,10 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>-0.1195959071778525</v>
+        <v>0.1195959071778525</v>
       </c>
       <c r="B59">
-        <v>-0.07963545357537179</v>
+        <v>0.07963545357537179</v>
       </c>
       <c r="C59">
         <v>-0.07301412264310475</v>
@@ -3650,10 +3650,10 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>-0.1186613703950178</v>
+        <v>0.1186613703950178</v>
       </c>
       <c r="B60">
-        <v>-0.08160723916976313</v>
+        <v>0.08160723916976313</v>
       </c>
       <c r="C60">
         <v>-0.0572661102574343</v>
@@ -3661,10 +3661,10 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>-0.1177437336621526</v>
+        <v>0.1177437336621526</v>
       </c>
       <c r="B61">
-        <v>-0.08319664562884668</v>
+        <v>0.08319664562884668</v>
       </c>
       <c r="C61">
         <v>-0.04076287030811893</v>
@@ -3672,10 +3672,10 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>-0.1168790803387934</v>
+        <v>0.1168790803387934</v>
       </c>
       <c r="B62">
-        <v>-0.08442267152091852</v>
+        <v>0.08442267152091852</v>
       </c>
       <c r="C62">
         <v>-0.02389231948148374</v>
@@ -3683,10 +3683,10 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>-0.1161240455792814</v>
+        <v>0.1161240455792814</v>
       </c>
       <c r="B63">
-        <v>-0.08533851809013374</v>
+        <v>0.08533851809013374</v>
       </c>
       <c r="C63">
         <v>-0.007013579311433635</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>-0.1155259607977101</v>
+        <v>0.1155259607977101</v>
       </c>
       <c r="B64">
-        <v>-0.0860185640497604</v>
+        <v>0.0860185640497604</v>
       </c>
       <c r="C64">
         <v>0.00953984716844245</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>-0.115108222334808</v>
+        <v>0.115108222334808</v>
       </c>
       <c r="B65">
-        <v>-0.08650878925114763</v>
+        <v>0.08650878925114763</v>
       </c>
       <c r="C65">
         <v>0.02546894761491289</v>
@@ -3716,10 +3716,10 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>-0.1148836371894487</v>
+        <v>0.1148836371894487</v>
       </c>
       <c r="B66">
-        <v>-0.08683576071084344</v>
+        <v>0.08683576071084344</v>
       </c>
       <c r="C66">
         <v>0.04051381324517576</v>
@@ -3727,10 +3727,10 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>-0.1148374077177494</v>
+        <v>0.1148374077177494</v>
       </c>
       <c r="B67">
-        <v>-0.08704661074287627</v>
+        <v>0.08704661074287627</v>
       </c>
       <c r="C67">
         <v>0.05450631767407476</v>
@@ -3738,10 +3738,10 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>-0.114940442365541</v>
+        <v>0.114940442365541</v>
       </c>
       <c r="B68">
-        <v>-0.08719619722812426</v>
+        <v>0.08719619722812426</v>
       </c>
       <c r="C68">
         <v>0.06735808984421601</v>
@@ -3749,10 +3749,10 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>-0.1151877634845399</v>
+        <v>0.1151877634845399</v>
       </c>
       <c r="B69">
-        <v>-0.08733026636333696</v>
+        <v>0.08733026636333696</v>
       </c>
       <c r="C69">
         <v>0.07902022387684671</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>-0.1155446847740357</v>
+        <v>0.1155446847740357</v>
       </c>
       <c r="B70">
-        <v>-0.08747990103078625</v>
+        <v>0.08747990103078625</v>
       </c>
       <c r="C70">
         <v>0.08944570250399832</v>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>-0.1159436866553981</v>
+        <v>0.1159436866553981</v>
       </c>
       <c r="B71">
-        <v>-0.08767923528711384</v>
+        <v>0.08767923528711384</v>
       </c>
       <c r="C71">
         <v>0.09858203572242984</v>
@@ -3782,10 +3782,10 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>-0.1163023727382986</v>
+        <v>0.1163023727382986</v>
       </c>
       <c r="B72">
-        <v>-0.08794912064420639</v>
+        <v>0.08794912064420639</v>
       </c>
       <c r="C72">
         <v>0.1064046634549001</v>
@@ -3793,10 +3793,10 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>-0.1165189832789967</v>
+        <v>0.1165189832789967</v>
       </c>
       <c r="B73">
-        <v>-0.08829840516434319</v>
+        <v>0.08829840516434319</v>
       </c>
       <c r="C73">
         <v>0.1129292581072973</v>
@@ -3804,10 +3804,10 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>-0.1164835223038357</v>
+        <v>0.1164835223038357</v>
       </c>
       <c r="B74">
-        <v>-0.08873402081478829</v>
+        <v>0.08873402081478829</v>
       </c>
       <c r="C74">
         <v>0.1181838707213976</v>
@@ -3815,10 +3815,10 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>-0.1161133585955221</v>
+        <v>0.1161133585955221</v>
       </c>
       <c r="B75">
-        <v>-0.08928742973560602</v>
+        <v>0.08928742973560602</v>
       </c>
       <c r="C75">
         <v>0.1222002304440462</v>
@@ -3826,10 +3826,10 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>-0.1153600326004128</v>
+        <v>0.1153600326004128</v>
       </c>
       <c r="B76">
-        <v>-0.08997515969433463</v>
+        <v>0.08997515969433463</v>
       </c>
       <c r="C76">
         <v>0.1249654630556118</v>
@@ -3837,10 +3837,10 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>-0.1142107508366547</v>
+        <v>0.1142107508366547</v>
       </c>
       <c r="B77">
-        <v>-0.09077937913561625</v>
+        <v>0.09077937913561625</v>
       </c>
       <c r="C77">
         <v>0.1264401806783723</v>
@@ -3848,10 +3848,10 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>-0.1126825682083056</v>
+        <v>0.1126825682083056</v>
       </c>
       <c r="B78">
-        <v>-0.09165682604283548</v>
+        <v>0.09165682604283548</v>
       </c>
       <c r="C78">
         <v>0.1266160259530763</v>
@@ -3859,10 +3859,10 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>-0.1107830033440867</v>
+        <v>0.1107830033440867</v>
       </c>
       <c r="B79">
-        <v>-0.09257780481077689</v>
+        <v>0.09257780481077689</v>
       </c>
       <c r="C79">
         <v>0.125503073832637</v>
@@ -3870,10 +3870,10 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>-0.1085055254543007</v>
+        <v>0.1085055254543007</v>
       </c>
       <c r="B80">
-        <v>-0.09352514736016554</v>
+        <v>0.09352514736016554</v>
       </c>
       <c r="C80">
         <v>0.123111794710043</v>
@@ -3881,10 +3881,10 @@
     </row>
     <row r="81">
       <c r="A81">
-        <v>-0.1058561845378069</v>
+        <v>0.1058561845378069</v>
       </c>
       <c r="B81">
-        <v>-0.094507625677008</v>
+        <v>0.094507625677008</v>
       </c>
       <c r="C81">
         <v>0.1194574380080261</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>-0.1029004326375739</v>
+        <v>0.1029004326375739</v>
       </c>
       <c r="B82">
-        <v>-0.09554210788087959</v>
+        <v>0.09554210788087959</v>
       </c>
       <c r="C82">
         <v>0.114543634239492</v>
@@ -3903,10 +3903,10 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>-0.09972660611048748</v>
+        <v>0.09972660611048748</v>
       </c>
       <c r="B83">
-        <v>-0.09663984972082268</v>
+        <v>0.09663984972082268</v>
       </c>
       <c r="C83">
         <v>0.1083706163286962</v>
@@ -3914,10 +3914,10 @@
     </row>
     <row r="84">
       <c r="A84">
-        <v>-0.09643932545921344</v>
+        <v>0.09643932545921344</v>
       </c>
       <c r="B84">
-        <v>-0.09782868661638794</v>
+        <v>0.09782868661638794</v>
       </c>
       <c r="C84">
         <v>0.1009346676710393</v>
@@ -3925,10 +3925,10 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>-0.09314302800540604</v>
+        <v>0.09314302800540604</v>
       </c>
       <c r="B85">
-        <v>-0.09911508118732211</v>
+        <v>0.09911508118732211</v>
       </c>
       <c r="C85">
         <v>0.09222578621432116</v>
@@ -3936,10 +3936,10 @@
     </row>
     <row r="86">
       <c r="A86">
-        <v>-0.08992726155678313</v>
+        <v>0.08992726155678313</v>
       </c>
       <c r="B86">
-        <v>-0.1004870424996145</v>
+        <v>0.1004870424996145</v>
       </c>
       <c r="C86">
         <v>0.08224025680597859</v>
@@ -3947,10 +3947,10 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>-0.08682759879198783</v>
+        <v>0.08682759879198783</v>
       </c>
       <c r="B87">
-        <v>-0.1019337996773496</v>
+        <v>0.1019337996773496</v>
       </c>
       <c r="C87">
         <v>0.07098458371014446</v>
@@ -3958,10 +3958,10 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>-0.08385223446502425</v>
+        <v>0.08385223446502425</v>
       </c>
       <c r="B88">
-        <v>-0.1034251543065126</v>
+        <v>0.1034251543065126</v>
       </c>
       <c r="C88">
         <v>0.05850556509518146</v>
@@ -3969,10 +3969,10 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>-0.08099213456433688</v>
+        <v>0.08099213456433688</v>
       </c>
       <c r="B89">
-        <v>-0.1049493052078773</v>
+        <v>0.1049493052078773</v>
       </c>
       <c r="C89">
         <v>0.04484646919265599</v>
@@ -3980,10 +3980,10 @@
     </row>
     <row r="90">
       <c r="A90">
-        <v>-0.07821112937253931</v>
+        <v>0.07821112937253931</v>
       </c>
       <c r="B90">
-        <v>-0.1064995318512713</v>
+        <v>0.1064995318512713</v>
       </c>
       <c r="C90">
         <v>0.03002327478951087</v>
@@ -3991,10 +3991,10 @@
     </row>
     <row r="91">
       <c r="A91">
-        <v>-0.07549164029096311</v>
+        <v>0.07549164029096311</v>
       </c>
       <c r="B91">
-        <v>-0.1080406142607434</v>
+        <v>0.1080406142607434</v>
       </c>
       <c r="C91">
         <v>0.0140110757383466</v>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="92">
       <c r="A92">
-        <v>-0.07282729820659282</v>
+        <v>0.07282729820659282</v>
       </c>
       <c r="B92">
-        <v>-0.1095374372967299</v>
+        <v>0.1095374372967299</v>
       </c>
       <c r="C92">
         <v>-0.003168391008868944</v>
@@ -4013,10 +4013,10 @@
     </row>
     <row r="93">
       <c r="A93">
-        <v>-0.07021113095952444</v>
+        <v>0.07021113095952444</v>
       </c>
       <c r="B93">
-        <v>-0.1109647936065532</v>
+        <v>0.1109647936065532</v>
       </c>
       <c r="C93">
         <v>-0.02144803826104346</v>
@@ -4024,10 +4024,10 @@
     </row>
     <row r="94">
       <c r="A94">
-        <v>-0.06762089429452042</v>
+        <v>0.06762089429452042</v>
       </c>
       <c r="B94">
-        <v>-0.112345955457771</v>
+        <v>0.112345955457771</v>
       </c>
       <c r="C94">
         <v>-0.04074270098908049</v>
@@ -4035,10 +4035,10 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>-0.06503739759682531</v>
+        <v>0.06503739759682531</v>
       </c>
       <c r="B95">
-        <v>-0.1137260557441816</v>
+        <v>0.1137260557441816</v>
       </c>
       <c r="C95">
         <v>-0.06090185040425431</v>
@@ -4046,10 +4046,10 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>-0.06243172487795604</v>
+        <v>0.06243172487795604</v>
       </c>
       <c r="B96">
-        <v>-0.1151703019371564</v>
+        <v>0.1151703019371564</v>
       </c>
       <c r="C96">
         <v>-0.08174312895249447</v>
@@ -4057,10 +4057,10 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>-0.0597821937546212</v>
+        <v>0.0597821937546212</v>
       </c>
       <c r="B97">
-        <v>-0.1167258112654936</v>
+        <v>0.1167258112654936</v>
       </c>
       <c r="C97">
         <v>-0.1030926656380046</v>
@@ -4068,10 +4068,10 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>-0.05709641232384591</v>
+        <v>0.05709641232384591</v>
       </c>
       <c r="B98">
-        <v>-0.1184114728822742</v>
+        <v>0.1184114728822742</v>
       </c>
       <c r="C98">
         <v>-0.1247984366025859</v>
@@ -4079,10 +4079,10 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>-0.05439349716927407</v>
+        <v>0.05439349716927407</v>
       </c>
       <c r="B99">
-        <v>-0.120247064547529</v>
+        <v>0.120247064547529</v>
       </c>
       <c r="C99">
         <v>-0.1467528425026699</v>
@@ -4090,10 +4090,10 @@
     </row>
     <row r="100">
       <c r="A100">
-        <v>-0.05169250713897352</v>
+        <v>0.05169250713897352</v>
       </c>
       <c r="B100">
-        <v>-0.1221997950482935</v>
+        <v>0.1221997950482935</v>
       </c>
       <c r="C100">
         <v>-0.1688494854745694</v>
@@ -4101,10 +4101,10 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>-0.04899273549016162</v>
+        <v>0.04899273549016162</v>
       </c>
       <c r="B101">
-        <v>-0.1242072483619488</v>
+        <v>0.1242072483619488</v>
       </c>
       <c r="C101">
         <v>-0.1909998643960533</v>
@@ -4112,10 +4112,10 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>-0.04628588245930788</v>
+        <v>0.04628588245930788</v>
       </c>
       <c r="B102">
-        <v>-0.1262396896588266</v>
+        <v>0.1262396896588266</v>
       </c>
       <c r="C102">
         <v>-0.2131636456649294</v>

</xml_diff>